<commit_message>
The following PR contains changes in cheklists links for English and French versions. I just inserted the base URL in the Spanish version but i guess it needs verification for example android 2.2
</commit_message>
<xml_diff>
--- a/Checklists/Mobile_App_Security_Checklist-English_1.1.xlsx
+++ b/Checklists/Mobile_App_Security_Checklist-English_1.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abderrahmane.LAPTOP-NBPOQCF6\Personal\R&amp;D\OWASP\MSTG\owasp-mstg\Checklists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FB55C9-0CBF-48B4-A1C8-147C15BF7372}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4B5966-7BEB-49E3-9D6D-0CBF0FBE7269}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="6" r:id="rId1"/>
@@ -2093,76 +2093,94 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2201,18 +2219,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2224,12 +2230,6 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="63">
@@ -3545,7 +3545,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:D48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A5" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="B12" sqref="B12:C12"/>
     </sheetView>
   </sheetViews>
@@ -3558,48 +3558,48 @@
   <sheetData>
     <row r="1" spans="2:4" ht="8" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="130" t="s">
         <v>220</v>
       </c>
-      <c r="C2" s="138"/>
-      <c r="D2" s="139"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="132"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B3" s="140"/>
-      <c r="C3" s="141"/>
-      <c r="D3" s="142"/>
+      <c r="B3" s="133"/>
+      <c r="C3" s="134"/>
+      <c r="D3" s="135"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="140"/>
-      <c r="C4" s="141"/>
-      <c r="D4" s="142"/>
+      <c r="B4" s="133"/>
+      <c r="C4" s="134"/>
+      <c r="D4" s="135"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="140"/>
-      <c r="C5" s="141"/>
-      <c r="D5" s="142"/>
+      <c r="B5" s="133"/>
+      <c r="C5" s="134"/>
+      <c r="D5" s="135"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B6" s="140"/>
-      <c r="C6" s="141"/>
-      <c r="D6" s="142"/>
+      <c r="B6" s="133"/>
+      <c r="C6" s="134"/>
+      <c r="D6" s="135"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B7" s="140"/>
-      <c r="C7" s="141"/>
-      <c r="D7" s="142"/>
+      <c r="B7" s="133"/>
+      <c r="C7" s="134"/>
+      <c r="D7" s="135"/>
     </row>
     <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="143"/>
-      <c r="C8" s="144"/>
-      <c r="D8" s="145"/>
+      <c r="B8" s="136"/>
+      <c r="C8" s="137"/>
+      <c r="D8" s="138"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B9" s="146" t="s">
+      <c r="B9" s="139" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="133"/>
-      <c r="D9" s="134"/>
+      <c r="C9" s="140"/>
+      <c r="D9" s="141"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
@@ -3609,19 +3609,19 @@
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B11" s="131" t="s">
+      <c r="B11" s="126" t="s">
         <v>221</v>
       </c>
-      <c r="C11" s="132"/>
+      <c r="C11" s="127"/>
       <c r="D11" s="12" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B12" s="171" t="s">
+      <c r="B12" s="145" t="s">
         <v>223</v>
       </c>
-      <c r="C12" s="172"/>
+      <c r="C12" s="146"/>
       <c r="D12" s="124" t="str">
         <f>HYPERLINK(CONCATENATE(
 "https://github.com/OWASP/owasp-mstg/blob/",
@@ -3631,69 +3631,69 @@
       </c>
     </row>
     <row r="13" spans="2:4" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="147" t="s">
+      <c r="B13" s="142" t="s">
         <v>265</v>
       </c>
-      <c r="C13" s="148"/>
-      <c r="D13" s="149"/>
+      <c r="C13" s="143"/>
+      <c r="D13" s="144"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B14" s="131" t="s">
+      <c r="B14" s="126" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="132"/>
+      <c r="C14" s="127"/>
       <c r="D14" s="12"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B15" s="126" t="s">
+      <c r="B15" s="128" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="136"/>
+      <c r="C15" s="129"/>
       <c r="D15" s="12"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B16" s="131" t="s">
+      <c r="B16" s="126" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="132"/>
+      <c r="C16" s="127"/>
       <c r="D16" s="12"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="131" t="s">
+      <c r="B17" s="126" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="132"/>
+      <c r="C17" s="127"/>
       <c r="D17" s="12"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="131" t="s">
+      <c r="B18" s="126" t="s">
         <v>135</v>
       </c>
-      <c r="C18" s="132"/>
+      <c r="C18" s="127"/>
       <c r="D18" s="12"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="131" t="s">
+      <c r="B19" s="126" t="s">
         <v>104</v>
       </c>
-      <c r="C19" s="132"/>
+      <c r="C19" s="127"/>
       <c r="D19" s="12" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="131" t="s">
+      <c r="B20" s="126" t="s">
         <v>106</v>
       </c>
-      <c r="C20" s="132"/>
+      <c r="C20" s="127"/>
       <c r="D20" s="12" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="133"/>
-      <c r="C21" s="133"/>
-      <c r="D21" s="134"/>
+      <c r="B21" s="140"/>
+      <c r="C21" s="140"/>
+      <c r="D21" s="141"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22" s="1" t="s">
@@ -3710,37 +3710,37 @@
       <c r="D23" s="12"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B24" s="131" t="s">
+      <c r="B24" s="126" t="s">
         <v>98</v>
       </c>
-      <c r="C24" s="132"/>
+      <c r="C24" s="127"/>
       <c r="D24" s="12"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B25" s="131" t="s">
+      <c r="B25" s="126" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="132"/>
+      <c r="C25" s="127"/>
       <c r="D25" s="12"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B26" s="131" t="s">
+      <c r="B26" s="126" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="132"/>
+      <c r="C26" s="127"/>
       <c r="D26" s="12"/>
     </row>
     <row r="27" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="135" t="s">
+      <c r="B27" s="151" t="s">
         <v>259</v>
       </c>
-      <c r="C27" s="132"/>
+      <c r="C27" s="127"/>
       <c r="D27" s="12"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B28" s="133"/>
-      <c r="C28" s="133"/>
-      <c r="D28" s="134"/>
+      <c r="B28" s="140"/>
+      <c r="C28" s="140"/>
+      <c r="D28" s="141"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B29" s="1" t="s">
@@ -3757,37 +3757,37 @@
       <c r="D30" s="12"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B31" s="131" t="s">
+      <c r="B31" s="126" t="s">
         <v>89</v>
       </c>
-      <c r="C31" s="132"/>
+      <c r="C31" s="127"/>
       <c r="D31" s="12"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B32" s="131" t="s">
+      <c r="B32" s="126" t="s">
         <v>99</v>
       </c>
-      <c r="C32" s="132"/>
+      <c r="C32" s="127"/>
       <c r="D32" s="12"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B33" s="131" t="s">
+      <c r="B33" s="126" t="s">
         <v>100</v>
       </c>
-      <c r="C33" s="132"/>
+      <c r="C33" s="127"/>
       <c r="D33" s="12"/>
     </row>
     <row r="34" spans="2:4" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="135" t="s">
+      <c r="B34" s="151" t="s">
         <v>260</v>
       </c>
-      <c r="C34" s="132"/>
+      <c r="C34" s="127"/>
       <c r="D34" s="12"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B35" s="133"/>
-      <c r="C35" s="133"/>
-      <c r="D35" s="134"/>
+      <c r="B35" s="140"/>
+      <c r="C35" s="140"/>
+      <c r="D35" s="141"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B36" s="1" t="s">
@@ -3797,98 +3797,97 @@
       <c r="D36" s="3"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B37" s="128"/>
-      <c r="C37" s="129"/>
-      <c r="D37" s="130"/>
+      <c r="B37" s="147"/>
+      <c r="C37" s="148"/>
+      <c r="D37" s="149"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B38" s="126" t="s">
+      <c r="B38" s="128" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="127"/>
+      <c r="C38" s="150"/>
       <c r="D38" s="39"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B39" s="126" t="s">
+      <c r="B39" s="128" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="127"/>
+      <c r="C39" s="150"/>
       <c r="D39" s="39"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B40" s="126" t="s">
+      <c r="B40" s="128" t="s">
         <v>93</v>
       </c>
-      <c r="C40" s="127"/>
+      <c r="C40" s="150"/>
       <c r="D40" s="39"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B41" s="126" t="s">
+      <c r="B41" s="128" t="s">
         <v>94</v>
       </c>
-      <c r="C41" s="127"/>
+      <c r="C41" s="150"/>
       <c r="D41" s="40"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B42" s="126" t="s">
+      <c r="B42" s="128" t="s">
         <v>95</v>
       </c>
-      <c r="C42" s="127"/>
+      <c r="C42" s="150"/>
       <c r="D42" s="39"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B43" s="128"/>
-      <c r="C43" s="129"/>
-      <c r="D43" s="130"/>
+      <c r="B43" s="147"/>
+      <c r="C43" s="148"/>
+      <c r="D43" s="149"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B44" s="126" t="s">
+      <c r="B44" s="128" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="127"/>
+      <c r="C44" s="150"/>
       <c r="D44" s="39"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B45" s="126" t="s">
+      <c r="B45" s="128" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="127"/>
+      <c r="C45" s="150"/>
       <c r="D45" s="39"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B46" s="126" t="s">
+      <c r="B46" s="128" t="s">
         <v>93</v>
       </c>
-      <c r="C46" s="127"/>
+      <c r="C46" s="150"/>
       <c r="D46" s="39"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B47" s="126" t="s">
+      <c r="B47" s="128" t="s">
         <v>94</v>
       </c>
-      <c r="C47" s="127"/>
+      <c r="C47" s="150"/>
       <c r="D47" s="40"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B48" s="126" t="s">
+      <c r="B48" s="128" t="s">
         <v>95</v>
       </c>
-      <c r="C48" s="127"/>
+      <c r="C48" s="150"/>
       <c r="D48" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B2:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:C44"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B37:D37"/>
@@ -3903,16 +3902,17 @@
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B2:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3959,11 +3959,11 @@
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="2:24" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="150"/>
-      <c r="C4" s="150"/>
-      <c r="D4" s="150"/>
-      <c r="E4" s="150"/>
-      <c r="F4" s="150"/>
+      <c r="B4" s="156"/>
+      <c r="C4" s="156"/>
+      <c r="D4" s="156"/>
+      <c r="E4" s="156"/>
+      <c r="F4" s="156"/>
     </row>
     <row r="5" spans="2:24" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="20"/>
@@ -3978,16 +3978,16 @@
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
-      <c r="G6" s="160" t="s">
+      <c r="G6" s="166" t="s">
         <v>117</v>
       </c>
-      <c r="H6" s="161"/>
-      <c r="I6" s="162"/>
-      <c r="V6" s="160" t="s">
+      <c r="H6" s="167"/>
+      <c r="I6" s="168"/>
+      <c r="V6" s="166" t="s">
         <v>117</v>
       </c>
-      <c r="W6" s="161"/>
-      <c r="X6" s="162"/>
+      <c r="W6" s="167"/>
+      <c r="X6" s="168"/>
     </row>
     <row r="7" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="13"/>
@@ -4002,18 +4002,18 @@
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
-      <c r="G8" s="151">
+      <c r="G8" s="157">
         <f>AVERAGE(G43:G50)*5</f>
         <v>0</v>
       </c>
-      <c r="H8" s="152"/>
-      <c r="I8" s="153"/>
-      <c r="V8" s="151">
+      <c r="H8" s="158"/>
+      <c r="I8" s="159"/>
+      <c r="V8" s="157">
         <f>AVERAGE(K43:K50)*5</f>
         <v>0</v>
       </c>
-      <c r="W8" s="152"/>
-      <c r="X8" s="153"/>
+      <c r="W8" s="158"/>
+      <c r="X8" s="159"/>
     </row>
     <row r="9" spans="2:24" ht="91" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="21"/>
@@ -4021,12 +4021,12 @@
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
-      <c r="G9" s="154"/>
-      <c r="H9" s="155"/>
-      <c r="I9" s="156"/>
-      <c r="V9" s="154"/>
-      <c r="W9" s="155"/>
-      <c r="X9" s="156"/>
+      <c r="G9" s="160"/>
+      <c r="H9" s="161"/>
+      <c r="I9" s="162"/>
+      <c r="V9" s="160"/>
+      <c r="W9" s="161"/>
+      <c r="X9" s="162"/>
     </row>
     <row r="10" spans="2:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="13"/>
@@ -4034,12 +4034,12 @@
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="154"/>
-      <c r="H10" s="155"/>
-      <c r="I10" s="156"/>
-      <c r="V10" s="154"/>
-      <c r="W10" s="155"/>
-      <c r="X10" s="156"/>
+      <c r="G10" s="160"/>
+      <c r="H10" s="161"/>
+      <c r="I10" s="162"/>
+      <c r="V10" s="160"/>
+      <c r="W10" s="161"/>
+      <c r="X10" s="162"/>
     </row>
     <row r="11" spans="2:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="13"/>
@@ -4047,19 +4047,19 @@
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="157"/>
-      <c r="H11" s="158"/>
-      <c r="I11" s="159"/>
-      <c r="V11" s="157"/>
-      <c r="W11" s="158"/>
-      <c r="X11" s="159"/>
+      <c r="G11" s="163"/>
+      <c r="H11" s="164"/>
+      <c r="I11" s="165"/>
+      <c r="V11" s="163"/>
+      <c r="W11" s="164"/>
+      <c r="X11" s="165"/>
     </row>
     <row r="12" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="163"/>
-      <c r="C12" s="163"/>
-      <c r="D12" s="163"/>
-      <c r="E12" s="163"/>
-      <c r="F12" s="163"/>
+      <c r="B12" s="152"/>
+      <c r="C12" s="152"/>
+      <c r="D12" s="152"/>
+      <c r="E12" s="152"/>
+      <c r="F12" s="152"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
@@ -4083,11 +4083,11 @@
       <c r="F15" s="13"/>
     </row>
     <row r="16" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="163"/>
-      <c r="C16" s="163"/>
-      <c r="D16" s="163"/>
-      <c r="E16" s="163"/>
-      <c r="F16" s="163"/>
+      <c r="B16" s="152"/>
+      <c r="C16" s="152"/>
+      <c r="D16" s="152"/>
+      <c r="E16" s="152"/>
+      <c r="F16" s="152"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="14"/>
@@ -4140,18 +4140,18 @@
     </row>
     <row r="35" spans="3:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="3:11" ht="14.5" x14ac:dyDescent="0.3">
-      <c r="D41" s="164" t="s">
+      <c r="D41" s="153" t="s">
         <v>115</v>
       </c>
-      <c r="E41" s="165"/>
-      <c r="F41" s="165"/>
-      <c r="G41" s="166"/>
-      <c r="H41" s="164" t="s">
+      <c r="E41" s="154"/>
+      <c r="F41" s="154"/>
+      <c r="G41" s="155"/>
+      <c r="H41" s="153" t="s">
         <v>116</v>
       </c>
-      <c r="I41" s="165"/>
-      <c r="J41" s="165"/>
-      <c r="K41" s="166"/>
+      <c r="I41" s="154"/>
+      <c r="J41" s="154"/>
+      <c r="K41" s="155"/>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.3">
       <c r="D42" s="17" t="s">
@@ -4477,6 +4477,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="V8:X11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="D41:G41"/>
@@ -4484,8 +4486,6 @@
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="G8:I11"/>
     <mergeCell ref="G6:I6"/>
-    <mergeCell ref="V6:X6"/>
-    <mergeCell ref="V8:X11"/>
   </mergeCells>
   <conditionalFormatting sqref="F14">
     <cfRule type="iconSet" priority="3">
@@ -4546,16 +4546,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B1" s="167" t="s">
+      <c r="B1" s="169" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="167"/>
-      <c r="I1" s="167"/>
+      <c r="C1" s="169"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="169"/>
+      <c r="F1" s="169"/>
+      <c r="G1" s="169"/>
+      <c r="H1" s="169"/>
+      <c r="I1" s="169"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="73"/>
@@ -4583,10 +4583,10 @@
       <c r="F3" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="G3" s="168" t="s">
+      <c r="G3" s="170" t="s">
         <v>273</v>
       </c>
-      <c r="H3" s="168"/>
+      <c r="H3" s="170"/>
       <c r="I3" s="113" t="s">
         <v>108</v>
       </c>
@@ -6818,10 +6818,10 @@
       <c r="F3" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="G3" s="168" t="s">
+      <c r="G3" s="170" t="s">
         <v>273</v>
       </c>
-      <c r="H3" s="169"/>
+      <c r="H3" s="171"/>
       <c r="I3" s="113" t="s">
         <v>108</v>
       </c>
@@ -9050,8 +9050,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A14" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -9062,10 +9062,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="170" t="s">
+      <c r="A1" s="172" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="170"/>
+      <c r="B1" s="172"/>
       <c r="C1" s="51"/>
       <c r="D1" s="33"/>
       <c r="E1" s="33"/>
@@ -9362,7 +9362,9 @@
       <c r="C20" s="50" t="s">
         <v>222</v>
       </c>
-      <c r="D20" s="43"/>
+      <c r="D20" s="43">
+        <v>43641</v>
+      </c>
       <c r="E20" s="92" t="s">
         <v>279</v>
       </c>

</xml_diff>

<commit_message>
the following PR contain changes in the links to MSTG based on OSS19 restructured chapters you can find details about the changes in the version history section. addition a link to the MASVS repo had been added.
</commit_message>
<xml_diff>
--- a/Checklists/Mobile_App_Security_Checklist-English_1.1.xlsx
+++ b/Checklists/Mobile_App_Security_Checklist-English_1.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abderrahmane.LAPTOP-NBPOQCF6\Personal\R&amp;D\OWASP\MSTG\owasp-mstg\Checklists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4B5966-7BEB-49E3-9D6D-0CBF0FBE7269}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFEF84E-0374-42F6-805A-2AC8CBEF2B2C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="6" r:id="rId1"/>
@@ -23,8 +23,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Security Requirements - Android'!$B$3:$I$72</definedName>
-    <definedName name="BASE_URL">Dashboard!$D$12</definedName>
+    <definedName name="BASE_URL">Dashboard!$D$14</definedName>
     <definedName name="MASVS_VERSION">Dashboard!$D$11</definedName>
+    <definedName name="MSTG_VERSION">Dashboard!$D$13</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="285">
   <si>
     <t>ID</t>
   </si>
@@ -719,9 +720,6 @@
       <t xml:space="preserve">
 Based on the OWASP Mobile Application Security Verification Standard</t>
     </r>
-  </si>
-  <si>
-    <t>MASVS Version:</t>
   </si>
   <si>
     <t>1.1.0</t>
@@ -1004,7 +1002,50 @@
     <t>1.1.1.1</t>
   </si>
   <si>
-    <t>Updating the links based on OSS19 restructured chapters</t>
+    <t>MSTG Version:</t>
+  </si>
+  <si>
+    <t>MASVS VERSION</t>
+  </si>
+  <si>
+    <t>1.1.4</t>
+  </si>
+  <si>
+    <t>Online version of the MASVS:</t>
+  </si>
+  <si>
+    <t>Correcting the Link to the MSTG repo and adding a link to the MASVS repo</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Updating the links based on OSS19 restructured chapters:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+android 
+3.2|3.4|4.9|4.10|5.2|5.4|7.7
+IOS
+3.2|4.5|4.10|4.11|5.1|5.3|6.4|7.8
+</t>
+    </r>
+  </si>
+  <si>
+    <t>1.1.1.2</t>
   </si>
 </sst>
 </file>
@@ -1325,7 +1366,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1724,6 +1765,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="63"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="63"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1790,7 +1842,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -2092,6 +2144,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -2140,6 +2207,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2149,11 +2222,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2170,6 +2240,42 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2183,42 +2289,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3543,376 +3613,400 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:D48"/>
+  <dimension ref="B1:D50"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:C12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
     <col min="4" max="4" width="92.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="8" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B2" s="130" t="s">
+      <c r="B2" s="135" t="s">
         <v>220</v>
       </c>
-      <c r="C2" s="131"/>
-      <c r="D2" s="132"/>
+      <c r="C2" s="136"/>
+      <c r="D2" s="137"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B3" s="133"/>
-      <c r="C3" s="134"/>
-      <c r="D3" s="135"/>
+      <c r="B3" s="138"/>
+      <c r="C3" s="139"/>
+      <c r="D3" s="140"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="133"/>
-      <c r="C4" s="134"/>
-      <c r="D4" s="135"/>
+      <c r="B4" s="138"/>
+      <c r="C4" s="139"/>
+      <c r="D4" s="140"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="133"/>
-      <c r="C5" s="134"/>
-      <c r="D5" s="135"/>
+      <c r="B5" s="138"/>
+      <c r="C5" s="139"/>
+      <c r="D5" s="140"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B6" s="133"/>
-      <c r="C6" s="134"/>
-      <c r="D6" s="135"/>
+      <c r="B6" s="138"/>
+      <c r="C6" s="139"/>
+      <c r="D6" s="140"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B7" s="133"/>
-      <c r="C7" s="134"/>
-      <c r="D7" s="135"/>
+      <c r="B7" s="138"/>
+      <c r="C7" s="139"/>
+      <c r="D7" s="140"/>
     </row>
     <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="136"/>
-      <c r="C8" s="137"/>
-      <c r="D8" s="138"/>
+      <c r="B8" s="141"/>
+      <c r="C8" s="142"/>
+      <c r="D8" s="143"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B9" s="139" t="s">
+      <c r="B9" s="144" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="140"/>
-      <c r="D9" s="141"/>
+      <c r="C9" s="145"/>
+      <c r="D9" s="146"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="126" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
+      <c r="C10" s="127"/>
+      <c r="D10" s="128"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B11" s="126" t="s">
-        <v>221</v>
-      </c>
-      <c r="C11" s="127"/>
-      <c r="D11" s="12" t="s">
-        <v>275</v>
+      <c r="B11" s="152" t="s">
+        <v>279</v>
+      </c>
+      <c r="C11" s="152"/>
+      <c r="D11" s="129" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B12" s="145" t="s">
-        <v>223</v>
-      </c>
-      <c r="C12" s="146"/>
-      <c r="D12" s="124" t="str">
-        <f>HYPERLINK(CONCATENATE(
-"https://github.com/OWASP/owasp-mstg/blob/",
+      <c r="B12" s="133" t="s">
+        <v>281</v>
+      </c>
+      <c r="C12" s="134"/>
+      <c r="D12" s="130" t="str">
+        <f>HYPERLINK(CONCATENATE(
+"https://github.com/OWASP/owasp-masvs/blob/",
 MASVS_VERSION,
 "/Document/"))</f>
+        <v>https://github.com/OWASP/owasp-masvs/blob/1.1.4/Document/</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B13" s="147" t="s">
+        <v>278</v>
+      </c>
+      <c r="C13" s="148"/>
+      <c r="D13" s="12" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B14" s="133" t="s">
+        <v>222</v>
+      </c>
+      <c r="C14" s="134"/>
+      <c r="D14" s="124" t="str">
+        <f>HYPERLINK(CONCATENATE(
+"https://github.com/OWASP/owasp-mstg/blob/",
+MSTG_VERSION,
+"/Document/"))</f>
         <v>https://github.com/OWASP/owasp-mstg/blob/1.1.2/Document/</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="142" t="s">
-        <v>265</v>
-      </c>
-      <c r="C13" s="143"/>
-      <c r="D13" s="144"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B14" s="126" t="s">
+    <row r="15" spans="2:4" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="149" t="s">
+        <v>264</v>
+      </c>
+      <c r="C15" s="150"/>
+      <c r="D15" s="151"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B16" s="131" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="127"/>
-      <c r="D14" s="12"/>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B15" s="128" t="s">
+      <c r="C16" s="132"/>
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B17" s="133" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="129"/>
-      <c r="D15" s="12"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B16" s="126" t="s">
+      <c r="C17" s="134"/>
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="131" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="127"/>
-      <c r="D16" s="12"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="126" t="s">
+      <c r="C18" s="132"/>
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B19" s="131" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="127"/>
-      <c r="D17" s="12"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="126" t="s">
+      <c r="C19" s="132"/>
+      <c r="D19" s="12"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B20" s="131" t="s">
         <v>135</v>
       </c>
-      <c r="C18" s="127"/>
-      <c r="D18" s="12"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="126" t="s">
+      <c r="C20" s="132"/>
+      <c r="D20" s="12"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B21" s="131" t="s">
         <v>104</v>
       </c>
-      <c r="C19" s="127"/>
-      <c r="D19" s="12" t="s">
+      <c r="C21" s="132"/>
+      <c r="D21" s="12" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="126" t="s">
+    <row r="22" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="131" t="s">
         <v>106</v>
       </c>
-      <c r="C20" s="127"/>
-      <c r="D20" s="12" t="s">
+      <c r="C22" s="132"/>
+      <c r="D22" s="12" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="140"/>
-      <c r="C21" s="140"/>
-      <c r="D21" s="141"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B22" s="1" t="s">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B23" s="145"/>
+      <c r="C23" s="145"/>
+      <c r="D23" s="146"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B24" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B23" s="4" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B25" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="12"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B24" s="126" t="s">
+      <c r="C25" s="5"/>
+      <c r="D25" s="12"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B26" s="131" t="s">
         <v>98</v>
       </c>
-      <c r="C24" s="127"/>
-      <c r="D24" s="12"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B25" s="126" t="s">
+      <c r="C26" s="132"/>
+      <c r="D26" s="12"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B27" s="131" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="127"/>
-      <c r="D25" s="12"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B26" s="126" t="s">
+      <c r="C27" s="132"/>
+      <c r="D27" s="12"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B28" s="131" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="127"/>
-      <c r="D26" s="12"/>
-    </row>
-    <row r="27" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="151" t="s">
+      <c r="C28" s="132"/>
+      <c r="D28" s="12"/>
+    </row>
+    <row r="29" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="157" t="s">
+        <v>258</v>
+      </c>
+      <c r="C29" s="132"/>
+      <c r="D29" s="12"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B30" s="145"/>
+      <c r="C30" s="145"/>
+      <c r="D30" s="146"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B31" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B32" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="49"/>
+      <c r="D32" s="12"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B33" s="131" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="132"/>
+      <c r="D33" s="12"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B34" s="131" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" s="132"/>
+      <c r="D34" s="12"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B35" s="131" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="132"/>
+      <c r="D35" s="12"/>
+    </row>
+    <row r="36" spans="2:4" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="157" t="s">
         <v>259</v>
       </c>
-      <c r="C27" s="127"/>
-      <c r="D27" s="12"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B28" s="140"/>
-      <c r="C28" s="140"/>
-      <c r="D28" s="141"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B29" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B30" s="48" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="49"/>
-      <c r="D30" s="12"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B31" s="126" t="s">
-        <v>89</v>
-      </c>
-      <c r="C31" s="127"/>
-      <c r="D31" s="12"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B32" s="126" t="s">
-        <v>99</v>
-      </c>
-      <c r="C32" s="127"/>
-      <c r="D32" s="12"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B33" s="126" t="s">
-        <v>100</v>
-      </c>
-      <c r="C33" s="127"/>
-      <c r="D33" s="12"/>
-    </row>
-    <row r="34" spans="2:4" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="151" t="s">
-        <v>260</v>
-      </c>
-      <c r="C34" s="127"/>
-      <c r="D34" s="12"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B35" s="140"/>
-      <c r="C35" s="140"/>
-      <c r="D35" s="141"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="132"/>
+      <c r="D36" s="12"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B37" s="145"/>
+      <c r="C37" s="145"/>
+      <c r="D37" s="146"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B38" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B37" s="147"/>
-      <c r="C37" s="148"/>
-      <c r="D37" s="149"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B38" s="128" t="s">
+      <c r="C38" s="2"/>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B39" s="153"/>
+      <c r="C39" s="154"/>
+      <c r="D39" s="155"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B40" s="133" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="150"/>
-      <c r="D38" s="39"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B39" s="128" t="s">
+      <c r="C40" s="156"/>
+      <c r="D40" s="39"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B41" s="133" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="150"/>
-      <c r="D39" s="39"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B40" s="128" t="s">
+      <c r="C41" s="156"/>
+      <c r="D41" s="39"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B42" s="133" t="s">
         <v>93</v>
       </c>
-      <c r="C40" s="150"/>
-      <c r="D40" s="39"/>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B41" s="128" t="s">
+      <c r="C42" s="156"/>
+      <c r="D42" s="39"/>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B43" s="133" t="s">
         <v>94</v>
       </c>
-      <c r="C41" s="150"/>
-      <c r="D41" s="40"/>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B42" s="128" t="s">
+      <c r="C43" s="156"/>
+      <c r="D43" s="40"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B44" s="133" t="s">
         <v>95</v>
       </c>
-      <c r="C42" s="150"/>
-      <c r="D42" s="39"/>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B43" s="147"/>
-      <c r="C43" s="148"/>
-      <c r="D43" s="149"/>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B44" s="128" t="s">
+      <c r="C44" s="156"/>
+      <c r="D44" s="39"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B45" s="153"/>
+      <c r="C45" s="154"/>
+      <c r="D45" s="155"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B46" s="133" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="150"/>
-      <c r="D44" s="39"/>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B45" s="128" t="s">
+      <c r="C46" s="156"/>
+      <c r="D46" s="39"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B47" s="133" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="150"/>
-      <c r="D45" s="39"/>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B46" s="128" t="s">
+      <c r="C47" s="156"/>
+      <c r="D47" s="39"/>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B48" s="133" t="s">
         <v>93</v>
       </c>
-      <c r="C46" s="150"/>
-      <c r="D46" s="39"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B47" s="128" t="s">
+      <c r="C48" s="156"/>
+      <c r="D48" s="39"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B49" s="133" t="s">
         <v>94</v>
       </c>
-      <c r="C47" s="150"/>
-      <c r="D47" s="40"/>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B48" s="128" t="s">
+      <c r="C49" s="156"/>
+      <c r="D49" s="40"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B50" s="133" t="s">
         <v>95</v>
       </c>
-      <c r="C48" s="150"/>
-      <c r="D48" s="39"/>
+      <c r="C50" s="156"/>
+      <c r="D50" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
+  <mergeCells count="37">
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B33:C33"/>
     <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B30:D30"/>
     <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
     <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B21:C21"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B15:C15"/>
     <mergeCell ref="B2:D8"/>
     <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3959,11 +4053,11 @@
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="2:24" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="156"/>
-      <c r="C4" s="156"/>
-      <c r="D4" s="156"/>
-      <c r="E4" s="156"/>
-      <c r="F4" s="156"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="174"/>
+      <c r="D4" s="174"/>
+      <c r="E4" s="174"/>
+      <c r="F4" s="174"/>
     </row>
     <row r="5" spans="2:24" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="20"/>
@@ -3978,16 +4072,16 @@
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
-      <c r="G6" s="166" t="s">
+      <c r="G6" s="158" t="s">
         <v>117</v>
       </c>
-      <c r="H6" s="167"/>
-      <c r="I6" s="168"/>
-      <c r="V6" s="166" t="s">
+      <c r="H6" s="159"/>
+      <c r="I6" s="160"/>
+      <c r="V6" s="158" t="s">
         <v>117</v>
       </c>
-      <c r="W6" s="167"/>
-      <c r="X6" s="168"/>
+      <c r="W6" s="159"/>
+      <c r="X6" s="160"/>
     </row>
     <row r="7" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="13"/>
@@ -4002,18 +4096,18 @@
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
-      <c r="G8" s="157">
+      <c r="G8" s="161">
         <f>AVERAGE(G43:G50)*5</f>
         <v>0</v>
       </c>
-      <c r="H8" s="158"/>
-      <c r="I8" s="159"/>
-      <c r="V8" s="157">
+      <c r="H8" s="162"/>
+      <c r="I8" s="163"/>
+      <c r="V8" s="161">
         <f>AVERAGE(K43:K50)*5</f>
         <v>0</v>
       </c>
-      <c r="W8" s="158"/>
-      <c r="X8" s="159"/>
+      <c r="W8" s="162"/>
+      <c r="X8" s="163"/>
     </row>
     <row r="9" spans="2:24" ht="91" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="21"/>
@@ -4021,12 +4115,12 @@
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
-      <c r="G9" s="160"/>
-      <c r="H9" s="161"/>
-      <c r="I9" s="162"/>
-      <c r="V9" s="160"/>
-      <c r="W9" s="161"/>
-      <c r="X9" s="162"/>
+      <c r="G9" s="164"/>
+      <c r="H9" s="165"/>
+      <c r="I9" s="166"/>
+      <c r="V9" s="164"/>
+      <c r="W9" s="165"/>
+      <c r="X9" s="166"/>
     </row>
     <row r="10" spans="2:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="13"/>
@@ -4034,12 +4128,12 @@
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="160"/>
-      <c r="H10" s="161"/>
-      <c r="I10" s="162"/>
-      <c r="V10" s="160"/>
-      <c r="W10" s="161"/>
-      <c r="X10" s="162"/>
+      <c r="G10" s="164"/>
+      <c r="H10" s="165"/>
+      <c r="I10" s="166"/>
+      <c r="V10" s="164"/>
+      <c r="W10" s="165"/>
+      <c r="X10" s="166"/>
     </row>
     <row r="11" spans="2:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="13"/>
@@ -4047,19 +4141,19 @@
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="163"/>
-      <c r="H11" s="164"/>
-      <c r="I11" s="165"/>
-      <c r="V11" s="163"/>
-      <c r="W11" s="164"/>
-      <c r="X11" s="165"/>
+      <c r="G11" s="167"/>
+      <c r="H11" s="168"/>
+      <c r="I11" s="169"/>
+      <c r="V11" s="167"/>
+      <c r="W11" s="168"/>
+      <c r="X11" s="169"/>
     </row>
     <row r="12" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="152"/>
-      <c r="C12" s="152"/>
-      <c r="D12" s="152"/>
-      <c r="E12" s="152"/>
-      <c r="F12" s="152"/>
+      <c r="B12" s="170"/>
+      <c r="C12" s="170"/>
+      <c r="D12" s="170"/>
+      <c r="E12" s="170"/>
+      <c r="F12" s="170"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
@@ -4083,11 +4177,11 @@
       <c r="F15" s="13"/>
     </row>
     <row r="16" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="152"/>
-      <c r="C16" s="152"/>
-      <c r="D16" s="152"/>
-      <c r="E16" s="152"/>
-      <c r="F16" s="152"/>
+      <c r="B16" s="170"/>
+      <c r="C16" s="170"/>
+      <c r="D16" s="170"/>
+      <c r="E16" s="170"/>
+      <c r="F16" s="170"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="14"/>
@@ -4140,18 +4234,18 @@
     </row>
     <row r="35" spans="3:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="3:11" ht="14.5" x14ac:dyDescent="0.3">
-      <c r="D41" s="153" t="s">
+      <c r="D41" s="171" t="s">
         <v>115</v>
       </c>
-      <c r="E41" s="154"/>
-      <c r="F41" s="154"/>
-      <c r="G41" s="155"/>
-      <c r="H41" s="153" t="s">
+      <c r="E41" s="172"/>
+      <c r="F41" s="172"/>
+      <c r="G41" s="173"/>
+      <c r="H41" s="171" t="s">
         <v>116</v>
       </c>
-      <c r="I41" s="154"/>
-      <c r="J41" s="154"/>
-      <c r="K41" s="155"/>
+      <c r="I41" s="172"/>
+      <c r="J41" s="172"/>
+      <c r="K41" s="173"/>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.3">
       <c r="D42" s="17" t="s">
@@ -4477,15 +4571,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G8:I11"/>
+    <mergeCell ref="G6:I6"/>
     <mergeCell ref="V6:X6"/>
     <mergeCell ref="V8:X11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="D41:G41"/>
     <mergeCell ref="H41:K41"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G8:I11"/>
-    <mergeCell ref="G6:I6"/>
   </mergeCells>
   <conditionalFormatting sqref="F14">
     <cfRule type="iconSet" priority="3">
@@ -4546,16 +4640,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B1" s="169" t="s">
+      <c r="B1" s="175" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="169"/>
-      <c r="D1" s="169"/>
-      <c r="E1" s="169"/>
-      <c r="F1" s="169"/>
-      <c r="G1" s="169"/>
-      <c r="H1" s="169"/>
-      <c r="I1" s="169"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="175"/>
+      <c r="H1" s="175"/>
+      <c r="I1" s="175"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="73"/>
@@ -4583,10 +4677,10 @@
       <c r="F3" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="G3" s="170" t="s">
-        <v>273</v>
-      </c>
-      <c r="H3" s="170"/>
+      <c r="G3" s="176" t="s">
+        <v>272</v>
+      </c>
+      <c r="H3" s="176"/>
       <c r="I3" s="113" t="s">
         <v>108</v>
       </c>
@@ -4627,7 +4721,7 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="70" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C6" s="109" t="s">
         <v>161</v>
@@ -4647,7 +4741,7 @@
     </row>
     <row r="7" spans="2:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="70" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C7" s="109" t="s">
         <v>162</v>
@@ -4667,7 +4761,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="70" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C8" s="109" t="s">
         <v>163</v>
@@ -4687,7 +4781,7 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B9" s="70" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C9" s="109" t="s">
         <v>164</v>
@@ -4707,7 +4801,7 @@
     </row>
     <row r="10" spans="2:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="70" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C10" s="109" t="s">
         <v>165</v>
@@ -4747,7 +4841,7 @@
     </row>
     <row r="12" spans="2:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B12" s="70" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C12" s="109" t="s">
         <v>167</v>
@@ -4767,7 +4861,7 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" s="70" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C13" s="109" t="s">
         <v>168</v>
@@ -5674,7 +5768,7 @@
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B53" s="71" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C53" s="110" t="s">
         <v>204</v>
@@ -5856,7 +5950,7 @@
     </row>
     <row r="61" spans="2:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B61" s="71" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C61" s="110" t="s">
         <v>150</v>
@@ -5880,7 +5974,7 @@
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B62" s="71" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C62" s="110" t="s">
         <v>211</v>
@@ -6370,10 +6464,10 @@
     </row>
     <row r="5" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="70" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C5" s="110" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>7</v>
@@ -6392,10 +6486,10 @@
     </row>
     <row r="6" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B6" s="70" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C6" s="110" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>7</v>
@@ -6415,10 +6509,10 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B7" s="70" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C7" s="110" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>7</v>
@@ -6437,10 +6531,10 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B8" s="70" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C8" s="110" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>7</v>
@@ -6459,10 +6553,10 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B9" s="70" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C9" s="110" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>7</v>
@@ -6481,10 +6575,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B10" s="70" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C10" s="110" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D10" s="24" t="s">
         <v>7</v>
@@ -6503,10 +6597,10 @@
     </row>
     <row r="11" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B11" s="70" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C11" s="110" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D11" s="24" t="s">
         <v>7</v>
@@ -6521,10 +6615,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B12" s="70" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C12" s="110" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>7</v>
@@ -6542,7 +6636,7 @@
         <v>155</v>
       </c>
       <c r="C13" s="110" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>7</v>
@@ -6574,7 +6668,7 @@
         <v>73</v>
       </c>
       <c r="C15" s="110" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D15" s="24" t="s">
         <v>7</v>
@@ -6603,10 +6697,10 @@
     </row>
     <row r="17" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B17" s="70" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C17" s="110" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D17" s="24" t="s">
         <v>7</v>
@@ -6625,10 +6719,10 @@
     </row>
     <row r="18" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="B18" s="70" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C18" s="110" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>7</v>
@@ -6818,10 +6912,10 @@
       <c r="F3" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="G3" s="170" t="s">
-        <v>273</v>
-      </c>
-      <c r="H3" s="171"/>
+      <c r="G3" s="176" t="s">
+        <v>272</v>
+      </c>
+      <c r="H3" s="177"/>
       <c r="I3" s="113" t="s">
         <v>108</v>
       </c>
@@ -6862,7 +6956,7 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="57" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C6" s="109" t="s">
         <v>161</v>
@@ -6882,7 +6976,7 @@
     </row>
     <row r="7" spans="2:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="57" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C7" s="109" t="s">
         <v>162</v>
@@ -6902,7 +6996,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="57" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C8" s="109" t="s">
         <v>163</v>
@@ -6922,7 +7016,7 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B9" s="57" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C9" s="109" t="s">
         <v>164</v>
@@ -6942,7 +7036,7 @@
     </row>
     <row r="10" spans="2:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="57" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C10" s="109" t="s">
         <v>165</v>
@@ -6982,7 +7076,7 @@
     </row>
     <row r="12" spans="2:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B12" s="57" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C12" s="109" t="s">
         <v>167</v>
@@ -7002,7 +7096,7 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" s="57" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C13" s="109" t="s">
         <v>168</v>
@@ -7923,7 +8017,7 @@
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B53" s="68" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C53" s="110" t="s">
         <v>204</v>
@@ -8105,7 +8199,7 @@
     </row>
     <row r="61" spans="2:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B61" s="68" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C61" s="110" t="s">
         <v>150</v>
@@ -8129,7 +8223,7 @@
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B62" s="68" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C62" s="110" t="s">
         <v>211</v>
@@ -8617,10 +8711,10 @@
     </row>
     <row r="5" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="70" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C5" s="110" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>7</v>
@@ -8639,10 +8733,10 @@
     </row>
     <row r="6" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B6" s="70" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C6" s="110" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>7</v>
@@ -8661,10 +8755,10 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B7" s="70" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C7" s="110" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>7</v>
@@ -8683,10 +8777,10 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B8" s="70" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C8" s="110" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>7</v>
@@ -8701,10 +8795,10 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B9" s="70" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C9" s="110" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>7</v>
@@ -8719,10 +8813,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B10" s="70" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C10" s="110" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D10" s="24" t="s">
         <v>7</v>
@@ -8737,10 +8831,10 @@
     </row>
     <row r="11" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B11" s="70" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C11" s="110" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D11" s="24" t="s">
         <v>7</v>
@@ -8755,10 +8849,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B12" s="70" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C12" s="110" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>7</v>
@@ -8776,7 +8870,7 @@
         <v>155</v>
       </c>
       <c r="C13" s="110" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>7</v>
@@ -8804,7 +8898,7 @@
         <v>73</v>
       </c>
       <c r="C15" s="110" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D15" s="24" t="s">
         <v>7</v>
@@ -8833,10 +8927,10 @@
     </row>
     <row r="17" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B17" s="70" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C17" s="110" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D17" s="24" t="s">
         <v>7</v>
@@ -8851,10 +8945,10 @@
     </row>
     <row r="18" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="B18" s="70" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C18" s="110" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>7</v>
@@ -9048,10 +9142,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -9062,10 +9156,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="172" t="s">
+      <c r="A1" s="178" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="172"/>
+      <c r="B1" s="178"/>
       <c r="C1" s="51"/>
       <c r="D1" s="33"/>
       <c r="E1" s="33"/>
@@ -9078,7 +9172,7 @@
         <v>100</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D2" s="44" t="s">
         <v>139</v>
@@ -9239,134 +9333,151 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="86" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B13" s="87" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C13" s="91"/>
       <c r="D13" s="88">
         <v>43464</v>
       </c>
       <c r="E13" s="89" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="86" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B14" s="87" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C14" s="91"/>
       <c r="D14" s="88">
         <v>43469</v>
       </c>
       <c r="E14" s="89" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="409" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="52" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D15" s="43">
         <v>43471</v>
       </c>
       <c r="E15" s="52" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="86" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B16" s="87" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D16" s="90">
         <v>43475</v>
       </c>
       <c r="E16" s="89" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A17" s="52" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B17" s="87" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D17" s="43">
         <v>43476</v>
       </c>
       <c r="E17" s="92" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A18" s="52" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B18" s="87" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D18" s="43">
         <v>43478</v>
       </c>
       <c r="E18" s="92" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A19" s="52" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B19" s="87" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C19" s="50" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D19" s="43">
         <v>43478</v>
       </c>
       <c r="E19" s="92" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A20" s="52" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B20" s="87" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C20" s="50" t="s">
-        <v>222</v>
+        <v>280</v>
       </c>
       <c r="D20" s="43">
         <v>43641</v>
       </c>
       <c r="E20" s="92" t="s">
-        <v>279</v>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="52" t="s">
+        <v>260</v>
+      </c>
+      <c r="B21" s="87" t="s">
+        <v>284</v>
+      </c>
+      <c r="C21" s="50" t="s">
+        <v>221</v>
+      </c>
+      <c r="D21" s="43">
+        <v>43642</v>
+      </c>
+      <c r="E21" s="92" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -9374,6 +9485,6 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
synchronizing the wording of each requirement in the excel files with the MASVS for the English and French versions
</commit_message>
<xml_diff>
--- a/Checklists/Mobile_App_Security_Checklist-English_1.1.xlsx
+++ b/Checklists/Mobile_App_Security_Checklist-English_1.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abderrahmane.LAPTOP-NBPOQCF6\Personal\R&amp;D\OWASP\MSTG\owasp-mstg\Checklists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFEF84E-0374-42F6-805A-2AC8CBEF2B2C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F248EFE2-2A85-4294-B2F1-B49AB9FA485A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="6" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="287">
   <si>
     <t>ID</t>
   </si>
@@ -579,9 +579,6 @@
   </si>
   <si>
     <t>No sensitive data is included in backups generated by the mobile operating system.</t>
-  </si>
-  <si>
-    <t>The app removes sensitive data from views when backgrounded.</t>
   </si>
   <si>
     <t>The app does not hold sensitive data in memory longer than necessary, and memory is cleared explicitly after use.</t>
@@ -1047,6 +1044,15 @@
   <si>
     <t>1.1.1.2</t>
   </si>
+  <si>
+    <t>The app removes sensitive data from views when moved to the background.</t>
+  </si>
+  <si>
+    <t>1.1.1.3</t>
+  </si>
+  <si>
+    <t>Synchronizing the requirements wording in excel with the MASVS</t>
+  </si>
 </sst>
 </file>
 
@@ -1055,9 +1061,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1779,527 +1792,533 @@
   </borders>
   <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="18" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="18" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="33" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="34" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="4" borderId="35" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="34" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="4" borderId="35" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="34" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="33" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="32" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="35" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="33" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="36" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="9" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="62" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="62" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="9" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="9" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="9" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="9" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="63">
@@ -3615,7 +3634,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:D50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -3628,48 +3647,48 @@
   <sheetData>
     <row r="1" spans="2:4" ht="8" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B2" s="135" t="s">
-        <v>220</v>
-      </c>
-      <c r="C2" s="136"/>
-      <c r="D2" s="137"/>
+      <c r="B2" s="142" t="s">
+        <v>219</v>
+      </c>
+      <c r="C2" s="143"/>
+      <c r="D2" s="144"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B3" s="138"/>
-      <c r="C3" s="139"/>
-      <c r="D3" s="140"/>
+      <c r="B3" s="145"/>
+      <c r="C3" s="146"/>
+      <c r="D3" s="147"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="138"/>
-      <c r="C4" s="139"/>
-      <c r="D4" s="140"/>
+      <c r="B4" s="145"/>
+      <c r="C4" s="146"/>
+      <c r="D4" s="147"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="138"/>
-      <c r="C5" s="139"/>
-      <c r="D5" s="140"/>
+      <c r="B5" s="145"/>
+      <c r="C5" s="146"/>
+      <c r="D5" s="147"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B6" s="138"/>
-      <c r="C6" s="139"/>
-      <c r="D6" s="140"/>
+      <c r="B6" s="145"/>
+      <c r="C6" s="146"/>
+      <c r="D6" s="147"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B7" s="138"/>
-      <c r="C7" s="139"/>
-      <c r="D7" s="140"/>
+      <c r="B7" s="145"/>
+      <c r="C7" s="146"/>
+      <c r="D7" s="147"/>
     </row>
     <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="141"/>
-      <c r="C8" s="142"/>
-      <c r="D8" s="143"/>
+      <c r="B8" s="148"/>
+      <c r="C8" s="149"/>
+      <c r="D8" s="150"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B9" s="144" t="s">
+      <c r="B9" s="151" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="145"/>
-      <c r="D9" s="146"/>
+      <c r="C9" s="138"/>
+      <c r="D9" s="139"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="126" t="s">
@@ -3679,19 +3698,19 @@
       <c r="D10" s="128"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B11" s="152" t="s">
+      <c r="B11" s="157" t="s">
+        <v>278</v>
+      </c>
+      <c r="C11" s="157"/>
+      <c r="D11" s="129" t="s">
         <v>279</v>
       </c>
-      <c r="C11" s="152"/>
-      <c r="D11" s="129" t="s">
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B12" s="131" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B12" s="133" t="s">
-        <v>281</v>
-      </c>
-      <c r="C12" s="134"/>
+      <c r="C12" s="141"/>
       <c r="D12" s="130" t="str">
         <f>HYPERLINK(CONCATENATE(
 "https://github.com/OWASP/owasp-masvs/blob/",
@@ -3701,19 +3720,19 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B13" s="147" t="s">
-        <v>278</v>
-      </c>
-      <c r="C13" s="148"/>
+      <c r="B13" s="152" t="s">
+        <v>277</v>
+      </c>
+      <c r="C13" s="153"/>
       <c r="D13" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B14" s="133" t="s">
-        <v>222</v>
-      </c>
-      <c r="C14" s="134"/>
+      <c r="B14" s="131" t="s">
+        <v>221</v>
+      </c>
+      <c r="C14" s="141"/>
       <c r="D14" s="124" t="str">
         <f>HYPERLINK(CONCATENATE(
 "https://github.com/OWASP/owasp-mstg/blob/",
@@ -3723,69 +3742,69 @@
       </c>
     </row>
     <row r="15" spans="2:4" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="149" t="s">
-        <v>264</v>
-      </c>
-      <c r="C15" s="150"/>
-      <c r="D15" s="151"/>
+      <c r="B15" s="154" t="s">
+        <v>263</v>
+      </c>
+      <c r="C15" s="155"/>
+      <c r="D15" s="156"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B16" s="131" t="s">
+      <c r="B16" s="136" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="132"/>
+      <c r="C16" s="137"/>
       <c r="D16" s="12"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="133" t="s">
+      <c r="B17" s="131" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="134"/>
+      <c r="C17" s="141"/>
       <c r="D17" s="12"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="131" t="s">
+      <c r="B18" s="136" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="132"/>
+      <c r="C18" s="137"/>
       <c r="D18" s="12"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="131" t="s">
+      <c r="B19" s="136" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="132"/>
+      <c r="C19" s="137"/>
       <c r="D19" s="12"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="131" t="s">
+      <c r="B20" s="136" t="s">
         <v>135</v>
       </c>
-      <c r="C20" s="132"/>
+      <c r="C20" s="137"/>
       <c r="D20" s="12"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="131" t="s">
+      <c r="B21" s="136" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="132"/>
+      <c r="C21" s="137"/>
       <c r="D21" s="12" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="131" t="s">
+      <c r="B22" s="136" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="132"/>
+      <c r="C22" s="137"/>
       <c r="D22" s="12" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B23" s="145"/>
-      <c r="C23" s="145"/>
-      <c r="D23" s="146"/>
+      <c r="B23" s="138"/>
+      <c r="C23" s="138"/>
+      <c r="D23" s="139"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
@@ -3802,37 +3821,37 @@
       <c r="D25" s="12"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B26" s="131" t="s">
+      <c r="B26" s="136" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="132"/>
+      <c r="C26" s="137"/>
       <c r="D26" s="12"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B27" s="131" t="s">
+      <c r="B27" s="136" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="132"/>
+      <c r="C27" s="137"/>
       <c r="D27" s="12"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B28" s="131" t="s">
+      <c r="B28" s="136" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="132"/>
+      <c r="C28" s="137"/>
       <c r="D28" s="12"/>
     </row>
     <row r="29" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="157" t="s">
-        <v>258</v>
-      </c>
-      <c r="C29" s="132"/>
+      <c r="B29" s="140" t="s">
+        <v>257</v>
+      </c>
+      <c r="C29" s="137"/>
       <c r="D29" s="12"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B30" s="145"/>
-      <c r="C30" s="145"/>
-      <c r="D30" s="146"/>
+      <c r="B30" s="138"/>
+      <c r="C30" s="138"/>
+      <c r="D30" s="139"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
@@ -3849,37 +3868,37 @@
       <c r="D32" s="12"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B33" s="131" t="s">
+      <c r="B33" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="132"/>
+      <c r="C33" s="137"/>
       <c r="D33" s="12"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B34" s="131" t="s">
+      <c r="B34" s="136" t="s">
         <v>99</v>
       </c>
-      <c r="C34" s="132"/>
+      <c r="C34" s="137"/>
       <c r="D34" s="12"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B35" s="131" t="s">
+      <c r="B35" s="136" t="s">
         <v>100</v>
       </c>
-      <c r="C35" s="132"/>
+      <c r="C35" s="137"/>
       <c r="D35" s="12"/>
     </row>
     <row r="36" spans="2:4" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="157" t="s">
-        <v>259</v>
-      </c>
-      <c r="C36" s="132"/>
+      <c r="B36" s="140" t="s">
+        <v>258</v>
+      </c>
+      <c r="C36" s="137"/>
       <c r="D36" s="12"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B37" s="145"/>
-      <c r="C37" s="145"/>
-      <c r="D37" s="146"/>
+      <c r="B37" s="138"/>
+      <c r="C37" s="138"/>
+      <c r="D37" s="139"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
@@ -3889,97 +3908,100 @@
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B39" s="153"/>
-      <c r="C39" s="154"/>
-      <c r="D39" s="155"/>
+      <c r="B39" s="133"/>
+      <c r="C39" s="134"/>
+      <c r="D39" s="135"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B40" s="133" t="s">
+      <c r="B40" s="131" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="156"/>
+      <c r="C40" s="132"/>
       <c r="D40" s="39"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B41" s="133" t="s">
+      <c r="B41" s="131" t="s">
         <v>92</v>
       </c>
-      <c r="C41" s="156"/>
+      <c r="C41" s="132"/>
       <c r="D41" s="39"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B42" s="133" t="s">
+      <c r="B42" s="131" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="156"/>
+      <c r="C42" s="132"/>
       <c r="D42" s="39"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B43" s="133" t="s">
+      <c r="B43" s="131" t="s">
         <v>94</v>
       </c>
-      <c r="C43" s="156"/>
+      <c r="C43" s="132"/>
       <c r="D43" s="40"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B44" s="133" t="s">
+      <c r="B44" s="131" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="156"/>
+      <c r="C44" s="132"/>
       <c r="D44" s="39"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B45" s="153"/>
-      <c r="C45" s="154"/>
-      <c r="D45" s="155"/>
+      <c r="B45" s="133"/>
+      <c r="C45" s="134"/>
+      <c r="D45" s="135"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B46" s="133" t="s">
+      <c r="B46" s="131" t="s">
         <v>91</v>
       </c>
-      <c r="C46" s="156"/>
+      <c r="C46" s="132"/>
       <c r="D46" s="39"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B47" s="133" t="s">
+      <c r="B47" s="131" t="s">
         <v>92</v>
       </c>
-      <c r="C47" s="156"/>
+      <c r="C47" s="132"/>
       <c r="D47" s="39"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B48" s="133" t="s">
+      <c r="B48" s="131" t="s">
         <v>93</v>
       </c>
-      <c r="C48" s="156"/>
+      <c r="C48" s="132"/>
       <c r="D48" s="39"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B49" s="133" t="s">
+      <c r="B49" s="131" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="156"/>
+      <c r="C49" s="132"/>
       <c r="D49" s="40"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B50" s="133" t="s">
+      <c r="B50" s="131" t="s">
         <v>95</v>
       </c>
-      <c r="C50" s="156"/>
+      <c r="C50" s="132"/>
       <c r="D50" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B2:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B39:D39"/>
@@ -3994,19 +4016,16 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B2:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:C46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4053,11 +4072,11 @@
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="2:24" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="174"/>
-      <c r="C4" s="174"/>
-      <c r="D4" s="174"/>
-      <c r="E4" s="174"/>
-      <c r="F4" s="174"/>
+      <c r="B4" s="158"/>
+      <c r="C4" s="158"/>
+      <c r="D4" s="158"/>
+      <c r="E4" s="158"/>
+      <c r="F4" s="158"/>
     </row>
     <row r="5" spans="2:24" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="20"/>
@@ -4072,16 +4091,16 @@
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
-      <c r="G6" s="158" t="s">
+      <c r="G6" s="168" t="s">
         <v>117</v>
       </c>
-      <c r="H6" s="159"/>
-      <c r="I6" s="160"/>
-      <c r="V6" s="158" t="s">
+      <c r="H6" s="169"/>
+      <c r="I6" s="170"/>
+      <c r="V6" s="168" t="s">
         <v>117</v>
       </c>
-      <c r="W6" s="159"/>
-      <c r="X6" s="160"/>
+      <c r="W6" s="169"/>
+      <c r="X6" s="170"/>
     </row>
     <row r="7" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="13"/>
@@ -4096,18 +4115,18 @@
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
-      <c r="G8" s="161">
+      <c r="G8" s="159">
         <f>AVERAGE(G43:G50)*5</f>
         <v>0</v>
       </c>
-      <c r="H8" s="162"/>
-      <c r="I8" s="163"/>
-      <c r="V8" s="161">
+      <c r="H8" s="160"/>
+      <c r="I8" s="161"/>
+      <c r="V8" s="159">
         <f>AVERAGE(K43:K50)*5</f>
         <v>0</v>
       </c>
-      <c r="W8" s="162"/>
-      <c r="X8" s="163"/>
+      <c r="W8" s="160"/>
+      <c r="X8" s="161"/>
     </row>
     <row r="9" spans="2:24" ht="91" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="21"/>
@@ -4115,12 +4134,12 @@
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
-      <c r="G9" s="164"/>
-      <c r="H9" s="165"/>
-      <c r="I9" s="166"/>
-      <c r="V9" s="164"/>
-      <c r="W9" s="165"/>
-      <c r="X9" s="166"/>
+      <c r="G9" s="162"/>
+      <c r="H9" s="163"/>
+      <c r="I9" s="164"/>
+      <c r="V9" s="162"/>
+      <c r="W9" s="163"/>
+      <c r="X9" s="164"/>
     </row>
     <row r="10" spans="2:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="13"/>
@@ -4128,12 +4147,12 @@
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="164"/>
-      <c r="H10" s="165"/>
-      <c r="I10" s="166"/>
-      <c r="V10" s="164"/>
-      <c r="W10" s="165"/>
-      <c r="X10" s="166"/>
+      <c r="G10" s="162"/>
+      <c r="H10" s="163"/>
+      <c r="I10" s="164"/>
+      <c r="V10" s="162"/>
+      <c r="W10" s="163"/>
+      <c r="X10" s="164"/>
     </row>
     <row r="11" spans="2:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="13"/>
@@ -4141,19 +4160,19 @@
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="167"/>
-      <c r="H11" s="168"/>
-      <c r="I11" s="169"/>
-      <c r="V11" s="167"/>
-      <c r="W11" s="168"/>
-      <c r="X11" s="169"/>
+      <c r="G11" s="165"/>
+      <c r="H11" s="166"/>
+      <c r="I11" s="167"/>
+      <c r="V11" s="165"/>
+      <c r="W11" s="166"/>
+      <c r="X11" s="167"/>
     </row>
     <row r="12" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="170"/>
-      <c r="C12" s="170"/>
-      <c r="D12" s="170"/>
-      <c r="E12" s="170"/>
-      <c r="F12" s="170"/>
+      <c r="B12" s="171"/>
+      <c r="C12" s="171"/>
+      <c r="D12" s="171"/>
+      <c r="E12" s="171"/>
+      <c r="F12" s="171"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
@@ -4177,11 +4196,11 @@
       <c r="F15" s="13"/>
     </row>
     <row r="16" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="170"/>
-      <c r="C16" s="170"/>
-      <c r="D16" s="170"/>
-      <c r="E16" s="170"/>
-      <c r="F16" s="170"/>
+      <c r="B16" s="171"/>
+      <c r="C16" s="171"/>
+      <c r="D16" s="171"/>
+      <c r="E16" s="171"/>
+      <c r="F16" s="171"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="14"/>
@@ -4234,18 +4253,18 @@
     </row>
     <row r="35" spans="3:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="3:11" ht="14.5" x14ac:dyDescent="0.3">
-      <c r="D41" s="171" t="s">
+      <c r="D41" s="172" t="s">
         <v>115</v>
       </c>
-      <c r="E41" s="172"/>
-      <c r="F41" s="172"/>
-      <c r="G41" s="173"/>
-      <c r="H41" s="171" t="s">
+      <c r="E41" s="173"/>
+      <c r="F41" s="173"/>
+      <c r="G41" s="174"/>
+      <c r="H41" s="172" t="s">
         <v>116</v>
       </c>
-      <c r="I41" s="172"/>
-      <c r="J41" s="172"/>
-      <c r="K41" s="173"/>
+      <c r="I41" s="173"/>
+      <c r="J41" s="173"/>
+      <c r="K41" s="174"/>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.3">
       <c r="D42" s="17" t="s">
@@ -4571,15 +4590,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="H41:K41"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="G8:I11"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="V6:X6"/>
     <mergeCell ref="V8:X11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="H41:K41"/>
   </mergeCells>
   <conditionalFormatting sqref="F14">
     <cfRule type="iconSet" priority="3">
@@ -4620,8 +4639,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:K85"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -4678,7 +4697,7 @@
         <v>107</v>
       </c>
       <c r="G3" s="176" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H3" s="176"/>
       <c r="I3" s="113" t="s">
@@ -4721,7 +4740,7 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="70" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C6" s="109" t="s">
         <v>161</v>
@@ -4741,7 +4760,7 @@
     </row>
     <row r="7" spans="2:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="70" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C7" s="109" t="s">
         <v>162</v>
@@ -4761,7 +4780,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="70" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C8" s="109" t="s">
         <v>163</v>
@@ -4781,7 +4800,7 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B9" s="70" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C9" s="109" t="s">
         <v>164</v>
@@ -4801,7 +4820,7 @@
     </row>
     <row r="10" spans="2:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="70" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C10" s="109" t="s">
         <v>165</v>
@@ -4841,7 +4860,7 @@
     </row>
     <row r="12" spans="2:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B12" s="70" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C12" s="109" t="s">
         <v>167</v>
@@ -4861,7 +4880,7 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" s="70" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C13" s="109" t="s">
         <v>168</v>
@@ -5009,7 +5028,7 @@
       <c r="B20" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="109" t="s">
+      <c r="C20" s="179" t="s">
         <v>174</v>
       </c>
       <c r="D20" s="25" t="s">
@@ -5033,7 +5052,7 @@
       <c r="B21" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="109" t="s">
+      <c r="C21" s="179" t="s">
         <v>175</v>
       </c>
       <c r="D21" s="25" t="s">
@@ -5057,7 +5076,7 @@
       <c r="B22" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="109" t="s">
+      <c r="C22" s="179" t="s">
         <v>176</v>
       </c>
       <c r="D22" s="25" t="s">
@@ -5081,7 +5100,7 @@
       <c r="B23" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="109" t="s">
+      <c r="C23" s="179" t="s">
         <v>177</v>
       </c>
       <c r="D23" s="37"/>
@@ -5105,8 +5124,8 @@
       <c r="B24" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="109" t="s">
-        <v>178</v>
+      <c r="C24" s="179" t="s">
+        <v>284</v>
       </c>
       <c r="D24" s="37"/>
       <c r="E24" s="34" t="s">
@@ -5129,8 +5148,8 @@
       <c r="B25" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="109" t="s">
-        <v>179</v>
+      <c r="C25" s="179" t="s">
+        <v>178</v>
       </c>
       <c r="D25" s="37"/>
       <c r="E25" s="34" t="s">
@@ -5153,8 +5172,8 @@
       <c r="B26" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="109" t="s">
-        <v>180</v>
+      <c r="C26" s="179" t="s">
+        <v>179</v>
       </c>
       <c r="D26" s="37"/>
       <c r="E26" s="34" t="s">
@@ -5178,7 +5197,7 @@
         <v>17</v>
       </c>
       <c r="C27" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D27" s="37"/>
       <c r="E27" s="34" t="s">
@@ -5215,8 +5234,8 @@
       <c r="B29" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="109" t="s">
-        <v>182</v>
+      <c r="C29" s="179" t="s">
+        <v>181</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>7</v>
@@ -5239,8 +5258,8 @@
       <c r="B30" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="109" t="s">
-        <v>183</v>
+      <c r="C30" s="179" t="s">
+        <v>182</v>
       </c>
       <c r="D30" s="25" t="s">
         <v>7</v>
@@ -5264,7 +5283,7 @@
         <v>21</v>
       </c>
       <c r="C31" s="109" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D31" s="25" t="s">
         <v>7</v>
@@ -5287,8 +5306,8 @@
       <c r="B32" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="109" t="s">
-        <v>185</v>
+      <c r="C32" s="179" t="s">
+        <v>184</v>
       </c>
       <c r="D32" s="25" t="s">
         <v>7</v>
@@ -5311,8 +5330,8 @@
       <c r="B33" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="109" t="s">
-        <v>186</v>
+      <c r="C33" s="179" t="s">
+        <v>185</v>
       </c>
       <c r="D33" s="25" t="s">
         <v>7</v>
@@ -5335,8 +5354,8 @@
       <c r="B34" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="109" t="s">
-        <v>187</v>
+      <c r="C34" s="179" t="s">
+        <v>186</v>
       </c>
       <c r="D34" s="25" t="s">
         <v>7</v>
@@ -5374,7 +5393,7 @@
         <v>26</v>
       </c>
       <c r="C36" s="110" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D36" s="25" t="s">
         <v>7</v>
@@ -5398,7 +5417,7 @@
         <v>55</v>
       </c>
       <c r="C37" s="110" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D37" s="25" t="s">
         <v>7</v>
@@ -5422,7 +5441,7 @@
         <v>56</v>
       </c>
       <c r="C38" s="110" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D38" s="25" t="s">
         <v>7</v>
@@ -5447,7 +5466,7 @@
         <v>27</v>
       </c>
       <c r="C39" s="110" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D39" s="25"/>
       <c r="E39" s="34"/>
@@ -5468,7 +5487,7 @@
         <v>28</v>
       </c>
       <c r="C40" s="110" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D40" s="25" t="s">
         <v>7</v>
@@ -5492,7 +5511,7 @@
         <v>57</v>
       </c>
       <c r="C41" s="110" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D41" s="25" t="s">
         <v>7</v>
@@ -5516,7 +5535,7 @@
         <v>58</v>
       </c>
       <c r="C42" s="110" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D42" s="25" t="s">
         <v>7</v>
@@ -5540,7 +5559,7 @@
         <v>29</v>
       </c>
       <c r="C43" s="110" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D43" s="37"/>
       <c r="E43" s="34" t="s">
@@ -5564,7 +5583,7 @@
         <v>30</v>
       </c>
       <c r="C44" s="110" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D44" s="37"/>
       <c r="E44" s="34" t="s">
@@ -5588,7 +5607,7 @@
         <v>31</v>
       </c>
       <c r="C45" s="110" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D45" s="37"/>
       <c r="E45" s="34" t="s">
@@ -5612,7 +5631,7 @@
         <v>151</v>
       </c>
       <c r="C46" s="110" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D46" s="37"/>
       <c r="E46" s="34" t="s">
@@ -5650,8 +5669,8 @@
       <c r="B48" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="C48" s="110" t="s">
-        <v>199</v>
+      <c r="C48" s="179" t="s">
+        <v>198</v>
       </c>
       <c r="D48" s="25" t="s">
         <v>7</v>
@@ -5675,7 +5694,7 @@
         <v>60</v>
       </c>
       <c r="C49" s="110" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D49" s="25" t="s">
         <v>7</v>
@@ -5699,7 +5718,7 @@
         <v>34</v>
       </c>
       <c r="C50" s="110" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D50" s="25" t="s">
         <v>7</v>
@@ -5723,7 +5742,7 @@
         <v>61</v>
       </c>
       <c r="C51" s="110" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D51" s="37"/>
       <c r="E51" s="34" t="s">
@@ -5747,7 +5766,7 @@
         <v>35</v>
       </c>
       <c r="C52" s="110" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D52" s="37"/>
       <c r="E52" s="34" t="s">
@@ -5768,10 +5787,10 @@
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B53" s="71" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C53" s="110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D53" s="37"/>
       <c r="E53" s="34" t="s">
@@ -5808,8 +5827,8 @@
       <c r="B55" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="C55" s="110" t="s">
-        <v>205</v>
+      <c r="C55" s="179" t="s">
+        <v>204</v>
       </c>
       <c r="D55" s="25" t="s">
         <v>7</v>
@@ -5833,7 +5852,7 @@
         <v>63</v>
       </c>
       <c r="C56" s="110" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D56" s="25" t="s">
         <v>7</v>
@@ -5856,8 +5875,8 @@
       <c r="B57" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="C57" s="110" t="s">
-        <v>207</v>
+      <c r="C57" s="179" t="s">
+        <v>206</v>
       </c>
       <c r="D57" s="25" t="s">
         <v>7</v>
@@ -5880,8 +5899,8 @@
       <c r="B58" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="C58" s="110" t="s">
-        <v>208</v>
+      <c r="C58" s="179" t="s">
+        <v>207</v>
       </c>
       <c r="D58" s="25" t="s">
         <v>7</v>
@@ -5904,8 +5923,8 @@
       <c r="B59" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="C59" s="110" t="s">
-        <v>209</v>
+      <c r="C59" s="179" t="s">
+        <v>208</v>
       </c>
       <c r="D59" s="25" t="s">
         <v>7</v>
@@ -5929,7 +5948,7 @@
         <v>67</v>
       </c>
       <c r="C60" s="110" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D60" s="25" t="s">
         <v>7</v>
@@ -5950,7 +5969,7 @@
     </row>
     <row r="61" spans="2:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B61" s="71" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C61" s="110" t="s">
         <v>150</v>
@@ -5974,10 +5993,10 @@
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B62" s="71" t="s">
-        <v>225</v>
-      </c>
-      <c r="C62" s="110" t="s">
-        <v>211</v>
+        <v>224</v>
+      </c>
+      <c r="C62" s="179" t="s">
+        <v>210</v>
       </c>
       <c r="D62" s="25" t="s">
         <v>7</v>
@@ -6014,8 +6033,8 @@
       <c r="B64" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="C64" s="109" t="s">
-        <v>212</v>
+      <c r="C64" s="179" t="s">
+        <v>211</v>
       </c>
       <c r="D64" s="25" t="s">
         <v>7</v>
@@ -6038,8 +6057,8 @@
       <c r="B65" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="C65" s="109" t="s">
-        <v>213</v>
+      <c r="C65" s="179" t="s">
+        <v>212</v>
       </c>
       <c r="D65" s="25" t="s">
         <v>7</v>
@@ -6062,8 +6081,8 @@
       <c r="B66" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="C66" s="109" t="s">
-        <v>214</v>
+      <c r="C66" s="179" t="s">
+        <v>213</v>
       </c>
       <c r="D66" s="25" t="s">
         <v>7</v>
@@ -6086,8 +6105,8 @@
       <c r="B67" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="C67" s="109" t="s">
-        <v>215</v>
+      <c r="C67" s="179" t="s">
+        <v>214</v>
       </c>
       <c r="D67" s="25" t="s">
         <v>7</v>
@@ -6111,7 +6130,7 @@
         <v>71</v>
       </c>
       <c r="C68" s="109" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D68" s="25" t="s">
         <v>7</v>
@@ -6134,8 +6153,8 @@
       <c r="B69" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="C69" s="109" t="s">
-        <v>217</v>
+      <c r="C69" s="179" t="s">
+        <v>216</v>
       </c>
       <c r="D69" s="25" t="s">
         <v>7</v>
@@ -6158,8 +6177,8 @@
       <c r="B70" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="C70" s="109" t="s">
-        <v>218</v>
+      <c r="C70" s="179" t="s">
+        <v>217</v>
       </c>
       <c r="D70" s="25" t="s">
         <v>7</v>
@@ -6182,8 +6201,8 @@
       <c r="B71" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="C71" s="109" t="s">
-        <v>219</v>
+      <c r="C71" s="179" t="s">
+        <v>218</v>
       </c>
       <c r="D71" s="25" t="s">
         <v>7</v>
@@ -6389,7 +6408,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6398,8 +6417,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B1:G29"/>
   <sheetViews>
-    <sheetView topLeftCell="B8" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="B10" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -6464,10 +6483,10 @@
     </row>
     <row r="5" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="70" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C5" s="110" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>7</v>
@@ -6486,10 +6505,10 @@
     </row>
     <row r="6" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B6" s="70" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C6" s="110" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>7</v>
@@ -6509,10 +6528,10 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B7" s="70" t="s">
-        <v>237</v>
-      </c>
-      <c r="C7" s="110" t="s">
-        <v>247</v>
+        <v>236</v>
+      </c>
+      <c r="C7" s="179" t="s">
+        <v>246</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>7</v>
@@ -6531,10 +6550,10 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B8" s="70" t="s">
-        <v>238</v>
-      </c>
-      <c r="C8" s="110" t="s">
-        <v>248</v>
+        <v>237</v>
+      </c>
+      <c r="C8" s="179" t="s">
+        <v>247</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>7</v>
@@ -6553,10 +6572,10 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B9" s="70" t="s">
-        <v>239</v>
-      </c>
-      <c r="C9" s="110" t="s">
-        <v>249</v>
+        <v>238</v>
+      </c>
+      <c r="C9" s="179" t="s">
+        <v>248</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>7</v>
@@ -6575,10 +6594,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B10" s="70" t="s">
-        <v>240</v>
-      </c>
-      <c r="C10" s="110" t="s">
-        <v>250</v>
+        <v>239</v>
+      </c>
+      <c r="C10" s="179" t="s">
+        <v>249</v>
       </c>
       <c r="D10" s="24" t="s">
         <v>7</v>
@@ -6597,10 +6616,10 @@
     </row>
     <row r="11" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B11" s="70" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C11" s="110" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D11" s="24" t="s">
         <v>7</v>
@@ -6615,10 +6634,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B12" s="70" t="s">
-        <v>242</v>
-      </c>
-      <c r="C12" s="110" t="s">
-        <v>252</v>
+        <v>241</v>
+      </c>
+      <c r="C12" s="179" t="s">
+        <v>251</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>7</v>
@@ -6635,8 +6654,8 @@
       <c r="B13" s="70" t="s">
         <v>155</v>
       </c>
-      <c r="C13" s="110" t="s">
-        <v>253</v>
+      <c r="C13" s="179" t="s">
+        <v>252</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>7</v>
@@ -6668,7 +6687,7 @@
         <v>73</v>
       </c>
       <c r="C15" s="110" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D15" s="24" t="s">
         <v>7</v>
@@ -6697,10 +6716,10 @@
     </row>
     <row r="17" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B17" s="70" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C17" s="110" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D17" s="24" t="s">
         <v>7</v>
@@ -6719,10 +6738,10 @@
     </row>
     <row r="18" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="B18" s="70" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C18" s="110" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>7</v>
@@ -6857,8 +6876,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:K85"/>
   <sheetViews>
-    <sheetView topLeftCell="D47" zoomScale="74" zoomScaleNormal="74" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView topLeftCell="A63" zoomScale="74" zoomScaleNormal="74" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -6913,7 +6932,7 @@
         <v>107</v>
       </c>
       <c r="G3" s="176" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H3" s="177"/>
       <c r="I3" s="113" t="s">
@@ -6956,7 +6975,7 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="57" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C6" s="109" t="s">
         <v>161</v>
@@ -6976,7 +6995,7 @@
     </row>
     <row r="7" spans="2:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="57" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C7" s="109" t="s">
         <v>162</v>
@@ -6996,7 +7015,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="57" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C8" s="109" t="s">
         <v>163</v>
@@ -7016,7 +7035,7 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B9" s="57" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C9" s="109" t="s">
         <v>164</v>
@@ -7036,7 +7055,7 @@
     </row>
     <row r="10" spans="2:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="57" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C10" s="109" t="s">
         <v>165</v>
@@ -7076,7 +7095,7 @@
     </row>
     <row r="12" spans="2:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B12" s="57" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C12" s="109" t="s">
         <v>167</v>
@@ -7096,7 +7115,7 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" s="57" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C13" s="109" t="s">
         <v>168</v>
@@ -7244,7 +7263,7 @@
       <c r="B20" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="109" t="s">
+      <c r="C20" s="179" t="s">
         <v>174</v>
       </c>
       <c r="D20" s="25" t="s">
@@ -7268,7 +7287,7 @@
       <c r="B21" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="109" t="s">
+      <c r="C21" s="179" t="s">
         <v>175</v>
       </c>
       <c r="D21" s="25" t="s">
@@ -7292,7 +7311,7 @@
       <c r="B22" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="109" t="s">
+      <c r="C22" s="179" t="s">
         <v>176</v>
       </c>
       <c r="D22" s="25" t="s">
@@ -7316,7 +7335,7 @@
       <c r="B23" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="109" t="s">
+      <c r="C23" s="179" t="s">
         <v>177</v>
       </c>
       <c r="D23" s="37"/>
@@ -7340,8 +7359,8 @@
       <c r="B24" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="109" t="s">
-        <v>178</v>
+      <c r="C24" s="179" t="s">
+        <v>284</v>
       </c>
       <c r="D24" s="37"/>
       <c r="E24" s="34" t="s">
@@ -7364,8 +7383,8 @@
       <c r="B25" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="109" t="s">
-        <v>179</v>
+      <c r="C25" s="179" t="s">
+        <v>178</v>
       </c>
       <c r="D25" s="37"/>
       <c r="E25" s="34" t="s">
@@ -7388,8 +7407,8 @@
       <c r="B26" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="109" t="s">
-        <v>180</v>
+      <c r="C26" s="179" t="s">
+        <v>179</v>
       </c>
       <c r="D26" s="37"/>
       <c r="E26" s="34" t="s">
@@ -7414,7 +7433,7 @@
         <v>17</v>
       </c>
       <c r="C27" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D27" s="37"/>
       <c r="E27" s="34" t="s">
@@ -7452,8 +7471,8 @@
       <c r="B29" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="109" t="s">
-        <v>182</v>
+      <c r="C29" s="179" t="s">
+        <v>181</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>7</v>
@@ -7476,8 +7495,8 @@
       <c r="B30" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="109" t="s">
-        <v>183</v>
+      <c r="C30" s="179" t="s">
+        <v>182</v>
       </c>
       <c r="D30" s="25" t="s">
         <v>7</v>
@@ -7501,7 +7520,7 @@
         <v>21</v>
       </c>
       <c r="C31" s="109" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D31" s="25" t="s">
         <v>7</v>
@@ -7524,8 +7543,8 @@
       <c r="B32" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="109" t="s">
-        <v>185</v>
+      <c r="C32" s="179" t="s">
+        <v>184</v>
       </c>
       <c r="D32" s="25" t="s">
         <v>7</v>
@@ -7548,8 +7567,8 @@
       <c r="B33" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="109" t="s">
-        <v>186</v>
+      <c r="C33" s="179" t="s">
+        <v>185</v>
       </c>
       <c r="D33" s="25" t="s">
         <v>7</v>
@@ -7572,8 +7591,8 @@
       <c r="B34" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="109" t="s">
-        <v>187</v>
+      <c r="C34" s="179" t="s">
+        <v>186</v>
       </c>
       <c r="D34" s="25" t="s">
         <v>7</v>
@@ -7611,7 +7630,7 @@
         <v>26</v>
       </c>
       <c r="C36" s="110" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D36" s="25" t="s">
         <v>7</v>
@@ -7635,7 +7654,7 @@
         <v>55</v>
       </c>
       <c r="C37" s="110" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D37" s="25" t="s">
         <v>7</v>
@@ -7659,7 +7678,7 @@
         <v>56</v>
       </c>
       <c r="C38" s="110" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D38" s="25" t="s">
         <v>7</v>
@@ -7683,7 +7702,7 @@
         <v>27</v>
       </c>
       <c r="C39" s="110" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D39" s="25"/>
       <c r="E39" s="34"/>
@@ -7705,7 +7724,7 @@
         <v>28</v>
       </c>
       <c r="C40" s="110" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D40" s="25" t="s">
         <v>7</v>
@@ -7730,7 +7749,7 @@
         <v>57</v>
       </c>
       <c r="C41" s="110" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D41" s="25" t="s">
         <v>7</v>
@@ -7754,7 +7773,7 @@
         <v>58</v>
       </c>
       <c r="C42" s="110" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D42" s="25" t="s">
         <v>7</v>
@@ -7778,7 +7797,7 @@
         <v>29</v>
       </c>
       <c r="C43" s="110" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D43" s="37"/>
       <c r="E43" s="34" t="s">
@@ -7802,7 +7821,7 @@
         <v>30</v>
       </c>
       <c r="C44" s="110" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D44" s="37"/>
       <c r="E44" s="34" t="s">
@@ -7826,7 +7845,7 @@
         <v>31</v>
       </c>
       <c r="C45" s="110" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D45" s="37"/>
       <c r="E45" s="34" t="s">
@@ -7850,7 +7869,7 @@
         <v>151</v>
       </c>
       <c r="C46" s="110" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D46" s="37"/>
       <c r="E46" s="34" t="s">
@@ -7887,8 +7906,8 @@
       <c r="B48" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="C48" s="110" t="s">
-        <v>199</v>
+      <c r="C48" s="179" t="s">
+        <v>198</v>
       </c>
       <c r="D48" s="25" t="s">
         <v>7</v>
@@ -7918,7 +7937,7 @@
         <v>60</v>
       </c>
       <c r="C49" s="110" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D49" s="25" t="s">
         <v>7</v>
@@ -7948,7 +7967,7 @@
         <v>34</v>
       </c>
       <c r="C50" s="110" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D50" s="25" t="s">
         <v>7</v>
@@ -7972,7 +7991,7 @@
         <v>61</v>
       </c>
       <c r="C51" s="110" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D51" s="37"/>
       <c r="E51" s="34" t="s">
@@ -7996,7 +8015,7 @@
         <v>35</v>
       </c>
       <c r="C52" s="110" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D52" s="37"/>
       <c r="E52" s="34" t="s">
@@ -8017,10 +8036,10 @@
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B53" s="68" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C53" s="110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D53" s="37"/>
       <c r="E53" s="34" t="s">
@@ -8057,8 +8076,8 @@
       <c r="B55" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="C55" s="110" t="s">
-        <v>205</v>
+      <c r="C55" s="179" t="s">
+        <v>204</v>
       </c>
       <c r="D55" s="25" t="s">
         <v>7</v>
@@ -8082,7 +8101,7 @@
         <v>63</v>
       </c>
       <c r="C56" s="110" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D56" s="25" t="s">
         <v>7</v>
@@ -8105,8 +8124,8 @@
       <c r="B57" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="C57" s="110" t="s">
-        <v>207</v>
+      <c r="C57" s="179" t="s">
+        <v>206</v>
       </c>
       <c r="D57" s="25" t="s">
         <v>7</v>
@@ -8129,8 +8148,8 @@
       <c r="B58" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="C58" s="110" t="s">
-        <v>208</v>
+      <c r="C58" s="179" t="s">
+        <v>207</v>
       </c>
       <c r="D58" s="25" t="s">
         <v>7</v>
@@ -8153,8 +8172,8 @@
       <c r="B59" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="C59" s="110" t="s">
-        <v>209</v>
+      <c r="C59" s="179" t="s">
+        <v>208</v>
       </c>
       <c r="D59" s="25" t="s">
         <v>7</v>
@@ -8178,7 +8197,7 @@
         <v>67</v>
       </c>
       <c r="C60" s="110" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D60" s="25" t="s">
         <v>7</v>
@@ -8199,7 +8218,7 @@
     </row>
     <row r="61" spans="2:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B61" s="68" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C61" s="110" t="s">
         <v>150</v>
@@ -8223,10 +8242,10 @@
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B62" s="68" t="s">
-        <v>225</v>
-      </c>
-      <c r="C62" s="110" t="s">
-        <v>211</v>
+        <v>224</v>
+      </c>
+      <c r="C62" s="179" t="s">
+        <v>210</v>
       </c>
       <c r="D62" s="25" t="s">
         <v>7</v>
@@ -8263,8 +8282,8 @@
       <c r="B64" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="C64" s="109" t="s">
-        <v>212</v>
+      <c r="C64" s="179" t="s">
+        <v>211</v>
       </c>
       <c r="D64" s="25" t="s">
         <v>7</v>
@@ -8287,8 +8306,8 @@
       <c r="B65" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="C65" s="109" t="s">
-        <v>213</v>
+      <c r="C65" s="179" t="s">
+        <v>212</v>
       </c>
       <c r="D65" s="25" t="s">
         <v>7</v>
@@ -8311,8 +8330,8 @@
       <c r="B66" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="C66" s="109" t="s">
-        <v>214</v>
+      <c r="C66" s="179" t="s">
+        <v>213</v>
       </c>
       <c r="D66" s="25" t="s">
         <v>7</v>
@@ -8335,8 +8354,8 @@
       <c r="B67" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="C67" s="109" t="s">
-        <v>215</v>
+      <c r="C67" s="179" t="s">
+        <v>214</v>
       </c>
       <c r="D67" s="25" t="s">
         <v>7</v>
@@ -8360,7 +8379,7 @@
         <v>71</v>
       </c>
       <c r="C68" s="109" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D68" s="25" t="s">
         <v>7</v>
@@ -8383,8 +8402,8 @@
       <c r="B69" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="C69" s="109" t="s">
-        <v>217</v>
+      <c r="C69" s="179" t="s">
+        <v>216</v>
       </c>
       <c r="D69" s="25" t="s">
         <v>7</v>
@@ -8407,8 +8426,8 @@
       <c r="B70" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="C70" s="109" t="s">
-        <v>218</v>
+      <c r="C70" s="179" t="s">
+        <v>217</v>
       </c>
       <c r="D70" s="25" t="s">
         <v>7</v>
@@ -8431,8 +8450,8 @@
       <c r="B71" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="C71" s="109" t="s">
-        <v>219</v>
+      <c r="C71" s="179" t="s">
+        <v>218</v>
       </c>
       <c r="D71" s="25" t="s">
         <v>7</v>
@@ -8655,7 +8674,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="B1:G32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -8711,10 +8730,10 @@
     </row>
     <row r="5" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="70" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C5" s="110" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>7</v>
@@ -8733,10 +8752,10 @@
     </row>
     <row r="6" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B6" s="70" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C6" s="110" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>7</v>
@@ -8755,10 +8774,10 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B7" s="70" t="s">
-        <v>237</v>
-      </c>
-      <c r="C7" s="110" t="s">
-        <v>247</v>
+        <v>236</v>
+      </c>
+      <c r="C7" s="179" t="s">
+        <v>246</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>7</v>
@@ -8777,10 +8796,10 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B8" s="70" t="s">
-        <v>238</v>
-      </c>
-      <c r="C8" s="110" t="s">
-        <v>248</v>
+        <v>237</v>
+      </c>
+      <c r="C8" s="179" t="s">
+        <v>247</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>7</v>
@@ -8795,10 +8814,10 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B9" s="70" t="s">
-        <v>239</v>
-      </c>
-      <c r="C9" s="110" t="s">
-        <v>249</v>
+        <v>238</v>
+      </c>
+      <c r="C9" s="179" t="s">
+        <v>248</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>7</v>
@@ -8813,10 +8832,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B10" s="70" t="s">
-        <v>240</v>
-      </c>
-      <c r="C10" s="110" t="s">
-        <v>250</v>
+        <v>239</v>
+      </c>
+      <c r="C10" s="179" t="s">
+        <v>249</v>
       </c>
       <c r="D10" s="24" t="s">
         <v>7</v>
@@ -8831,10 +8850,10 @@
     </row>
     <row r="11" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B11" s="70" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C11" s="110" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D11" s="24" t="s">
         <v>7</v>
@@ -8849,10 +8868,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B12" s="70" t="s">
-        <v>242</v>
-      </c>
-      <c r="C12" s="110" t="s">
-        <v>252</v>
+        <v>241</v>
+      </c>
+      <c r="C12" s="179" t="s">
+        <v>251</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>7</v>
@@ -8869,8 +8888,8 @@
       <c r="B13" s="70" t="s">
         <v>155</v>
       </c>
-      <c r="C13" s="110" t="s">
-        <v>253</v>
+      <c r="C13" s="179" t="s">
+        <v>252</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>7</v>
@@ -8898,7 +8917,7 @@
         <v>73</v>
       </c>
       <c r="C15" s="110" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D15" s="24" t="s">
         <v>7</v>
@@ -8927,10 +8946,10 @@
     </row>
     <row r="17" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B17" s="70" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C17" s="110" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D17" s="24" t="s">
         <v>7</v>
@@ -8945,10 +8964,10 @@
     </row>
     <row r="18" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="B18" s="70" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C18" s="110" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>7</v>
@@ -9142,10 +9161,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A16" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -9172,7 +9191,7 @@
         <v>100</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D2" s="44" t="s">
         <v>139</v>
@@ -9333,151 +9352,168 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="86" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B13" s="87" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C13" s="91"/>
       <c r="D13" s="88">
         <v>43464</v>
       </c>
       <c r="E13" s="89" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="86" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B14" s="87" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C14" s="91"/>
       <c r="D14" s="88">
         <v>43469</v>
       </c>
       <c r="E14" s="89" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="409" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="52" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D15" s="43">
         <v>43471</v>
       </c>
       <c r="E15" s="52" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="86" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B16" s="87" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D16" s="90">
         <v>43475</v>
       </c>
       <c r="E16" s="89" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A17" s="52" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B17" s="87" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D17" s="43">
         <v>43476</v>
       </c>
       <c r="E17" s="92" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A18" s="52" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B18" s="87" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D18" s="43">
         <v>43478</v>
       </c>
       <c r="E18" s="92" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A19" s="52" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B19" s="87" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C19" s="50" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D19" s="43">
         <v>43478</v>
       </c>
       <c r="E19" s="92" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A20" s="52" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B20" s="87" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C20" s="50" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D20" s="43">
         <v>43641</v>
       </c>
       <c r="E20" s="92" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="52" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B21" s="87" t="s">
-        <v>284</v>
-      </c>
-      <c r="C21" s="50" t="s">
-        <v>221</v>
+        <v>283</v>
+      </c>
+      <c r="C21" s="180" t="s">
+        <v>279</v>
       </c>
       <c r="D21" s="43">
         <v>43642</v>
       </c>
       <c r="E21" s="92" t="s">
-        <v>282</v>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="52" t="s">
+        <v>259</v>
+      </c>
+      <c r="B22" s="87" t="s">
+        <v>285</v>
+      </c>
+      <c r="C22" s="180" t="s">
+        <v>279</v>
+      </c>
+      <c r="D22" s="43">
+        <v>43645</v>
+      </c>
+      <c r="E22" s="92" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
synchronizing the wording of each requirement in the excel files with the MASVS for the English and the French versions
</commit_message>
<xml_diff>
--- a/Checklists/Mobile_App_Security_Checklist-English_1.1.xlsx
+++ b/Checklists/Mobile_App_Security_Checklist-English_1.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abderrahmane.LAPTOP-NBPOQCF6\Personal\R&amp;D\OWASP\MSTG\owasp-mstg\Checklists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F248EFE2-2A85-4294-B2F1-B49AB9FA485A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606517CC-7B3F-4EA8-B83A-2500B9593DC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="6" r:id="rId1"/>
@@ -1051,7 +1051,9 @@
     <t>1.1.1.3</t>
   </si>
   <si>
-    <t>Synchronizing the requirements wording in excel with the MASVS</t>
+    <t>Synchronizing the requirements wording in excel with the MASVS
+changes:
+2.9</t>
   </si>
 </sst>
 </file>
@@ -2172,86 +2174,104 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2290,18 +2310,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2313,12 +2321,6 @@
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="63">
@@ -3647,48 +3649,48 @@
   <sheetData>
     <row r="1" spans="2:4" ht="8" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B2" s="142" t="s">
+      <c r="B2" s="137" t="s">
         <v>219</v>
       </c>
-      <c r="C2" s="143"/>
-      <c r="D2" s="144"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="139"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B3" s="145"/>
-      <c r="C3" s="146"/>
-      <c r="D3" s="147"/>
+      <c r="B3" s="140"/>
+      <c r="C3" s="141"/>
+      <c r="D3" s="142"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="145"/>
-      <c r="C4" s="146"/>
-      <c r="D4" s="147"/>
+      <c r="B4" s="140"/>
+      <c r="C4" s="141"/>
+      <c r="D4" s="142"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="145"/>
-      <c r="C5" s="146"/>
-      <c r="D5" s="147"/>
+      <c r="B5" s="140"/>
+      <c r="C5" s="141"/>
+      <c r="D5" s="142"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B6" s="145"/>
-      <c r="C6" s="146"/>
-      <c r="D6" s="147"/>
+      <c r="B6" s="140"/>
+      <c r="C6" s="141"/>
+      <c r="D6" s="142"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B7" s="145"/>
-      <c r="C7" s="146"/>
-      <c r="D7" s="147"/>
+      <c r="B7" s="140"/>
+      <c r="C7" s="141"/>
+      <c r="D7" s="142"/>
     </row>
     <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="148"/>
-      <c r="C8" s="149"/>
-      <c r="D8" s="150"/>
+      <c r="B8" s="143"/>
+      <c r="C8" s="144"/>
+      <c r="D8" s="145"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B9" s="151" t="s">
+      <c r="B9" s="146" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="138"/>
-      <c r="D9" s="139"/>
+      <c r="C9" s="147"/>
+      <c r="D9" s="148"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="126" t="s">
@@ -3698,19 +3700,19 @@
       <c r="D10" s="128"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B11" s="157" t="s">
+      <c r="B11" s="154" t="s">
         <v>278</v>
       </c>
-      <c r="C11" s="157"/>
+      <c r="C11" s="154"/>
       <c r="D11" s="129" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B12" s="131" t="s">
+      <c r="B12" s="135" t="s">
         <v>280</v>
       </c>
-      <c r="C12" s="141"/>
+      <c r="C12" s="136"/>
       <c r="D12" s="130" t="str">
         <f>HYPERLINK(CONCATENATE(
 "https://github.com/OWASP/owasp-masvs/blob/",
@@ -3720,19 +3722,19 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B13" s="152" t="s">
+      <c r="B13" s="149" t="s">
         <v>277</v>
       </c>
-      <c r="C13" s="153"/>
+      <c r="C13" s="150"/>
       <c r="D13" s="12" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B14" s="131" t="s">
+      <c r="B14" s="135" t="s">
         <v>221</v>
       </c>
-      <c r="C14" s="141"/>
+      <c r="C14" s="136"/>
       <c r="D14" s="124" t="str">
         <f>HYPERLINK(CONCATENATE(
 "https://github.com/OWASP/owasp-mstg/blob/",
@@ -3742,69 +3744,69 @@
       </c>
     </row>
     <row r="15" spans="2:4" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="154" t="s">
+      <c r="B15" s="151" t="s">
         <v>263</v>
       </c>
-      <c r="C15" s="155"/>
-      <c r="D15" s="156"/>
+      <c r="C15" s="152"/>
+      <c r="D15" s="153"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B16" s="136" t="s">
+      <c r="B16" s="133" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="137"/>
+      <c r="C16" s="134"/>
       <c r="D16" s="12"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="131" t="s">
+      <c r="B17" s="135" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="141"/>
+      <c r="C17" s="136"/>
       <c r="D17" s="12"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="136" t="s">
+      <c r="B18" s="133" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="137"/>
+      <c r="C18" s="134"/>
       <c r="D18" s="12"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="136" t="s">
+      <c r="B19" s="133" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="137"/>
+      <c r="C19" s="134"/>
       <c r="D19" s="12"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="136" t="s">
+      <c r="B20" s="133" t="s">
         <v>135</v>
       </c>
-      <c r="C20" s="137"/>
+      <c r="C20" s="134"/>
       <c r="D20" s="12"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="136" t="s">
+      <c r="B21" s="133" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="137"/>
+      <c r="C21" s="134"/>
       <c r="D21" s="12" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="136" t="s">
+      <c r="B22" s="133" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="137"/>
+      <c r="C22" s="134"/>
       <c r="D22" s="12" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B23" s="138"/>
-      <c r="C23" s="138"/>
-      <c r="D23" s="139"/>
+      <c r="B23" s="147"/>
+      <c r="C23" s="147"/>
+      <c r="D23" s="148"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
@@ -3821,37 +3823,37 @@
       <c r="D25" s="12"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B26" s="136" t="s">
+      <c r="B26" s="133" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="137"/>
+      <c r="C26" s="134"/>
       <c r="D26" s="12"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B27" s="136" t="s">
+      <c r="B27" s="133" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="137"/>
+      <c r="C27" s="134"/>
       <c r="D27" s="12"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B28" s="136" t="s">
+      <c r="B28" s="133" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="137"/>
+      <c r="C28" s="134"/>
       <c r="D28" s="12"/>
     </row>
     <row r="29" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="140" t="s">
+      <c r="B29" s="159" t="s">
         <v>257</v>
       </c>
-      <c r="C29" s="137"/>
+      <c r="C29" s="134"/>
       <c r="D29" s="12"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B30" s="138"/>
-      <c r="C30" s="138"/>
-      <c r="D30" s="139"/>
+      <c r="B30" s="147"/>
+      <c r="C30" s="147"/>
+      <c r="D30" s="148"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
@@ -3868,37 +3870,37 @@
       <c r="D32" s="12"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B33" s="136" t="s">
+      <c r="B33" s="133" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="137"/>
+      <c r="C33" s="134"/>
       <c r="D33" s="12"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B34" s="136" t="s">
+      <c r="B34" s="133" t="s">
         <v>99</v>
       </c>
-      <c r="C34" s="137"/>
+      <c r="C34" s="134"/>
       <c r="D34" s="12"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B35" s="136" t="s">
+      <c r="B35" s="133" t="s">
         <v>100</v>
       </c>
-      <c r="C35" s="137"/>
+      <c r="C35" s="134"/>
       <c r="D35" s="12"/>
     </row>
     <row r="36" spans="2:4" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="140" t="s">
+      <c r="B36" s="159" t="s">
         <v>258</v>
       </c>
-      <c r="C36" s="137"/>
+      <c r="C36" s="134"/>
       <c r="D36" s="12"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B37" s="138"/>
-      <c r="C37" s="138"/>
-      <c r="D37" s="139"/>
+      <c r="B37" s="147"/>
+      <c r="C37" s="147"/>
+      <c r="D37" s="148"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
@@ -3908,100 +3910,97 @@
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B39" s="133"/>
-      <c r="C39" s="134"/>
-      <c r="D39" s="135"/>
+      <c r="B39" s="155"/>
+      <c r="C39" s="156"/>
+      <c r="D39" s="157"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B40" s="131" t="s">
+      <c r="B40" s="135" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="132"/>
+      <c r="C40" s="158"/>
       <c r="D40" s="39"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B41" s="131" t="s">
+      <c r="B41" s="135" t="s">
         <v>92</v>
       </c>
-      <c r="C41" s="132"/>
+      <c r="C41" s="158"/>
       <c r="D41" s="39"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B42" s="131" t="s">
+      <c r="B42" s="135" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="132"/>
+      <c r="C42" s="158"/>
       <c r="D42" s="39"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B43" s="131" t="s">
+      <c r="B43" s="135" t="s">
         <v>94</v>
       </c>
-      <c r="C43" s="132"/>
+      <c r="C43" s="158"/>
       <c r="D43" s="40"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B44" s="131" t="s">
+      <c r="B44" s="135" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="132"/>
+      <c r="C44" s="158"/>
       <c r="D44" s="39"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B45" s="133"/>
-      <c r="C45" s="134"/>
-      <c r="D45" s="135"/>
+      <c r="B45" s="155"/>
+      <c r="C45" s="156"/>
+      <c r="D45" s="157"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B46" s="131" t="s">
+      <c r="B46" s="135" t="s">
         <v>91</v>
       </c>
-      <c r="C46" s="132"/>
+      <c r="C46" s="158"/>
       <c r="D46" s="39"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B47" s="131" t="s">
+      <c r="B47" s="135" t="s">
         <v>92</v>
       </c>
-      <c r="C47" s="132"/>
+      <c r="C47" s="158"/>
       <c r="D47" s="39"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B48" s="131" t="s">
+      <c r="B48" s="135" t="s">
         <v>93</v>
       </c>
-      <c r="C48" s="132"/>
+      <c r="C48" s="158"/>
       <c r="D48" s="39"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B49" s="131" t="s">
+      <c r="B49" s="135" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="132"/>
+      <c r="C49" s="158"/>
       <c r="D49" s="40"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B50" s="131" t="s">
+      <c r="B50" s="135" t="s">
         <v>95</v>
       </c>
-      <c r="C50" s="132"/>
+      <c r="C50" s="158"/>
       <c r="D50" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B2:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:C46"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B39:D39"/>
@@ -4016,16 +4015,19 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B2:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4072,11 +4074,11 @@
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="2:24" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="158"/>
-      <c r="C4" s="158"/>
-      <c r="D4" s="158"/>
-      <c r="E4" s="158"/>
-      <c r="F4" s="158"/>
+      <c r="B4" s="164"/>
+      <c r="C4" s="164"/>
+      <c r="D4" s="164"/>
+      <c r="E4" s="164"/>
+      <c r="F4" s="164"/>
     </row>
     <row r="5" spans="2:24" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="20"/>
@@ -4091,16 +4093,16 @@
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
-      <c r="G6" s="168" t="s">
+      <c r="G6" s="174" t="s">
         <v>117</v>
       </c>
-      <c r="H6" s="169"/>
-      <c r="I6" s="170"/>
-      <c r="V6" s="168" t="s">
+      <c r="H6" s="175"/>
+      <c r="I6" s="176"/>
+      <c r="V6" s="174" t="s">
         <v>117</v>
       </c>
-      <c r="W6" s="169"/>
-      <c r="X6" s="170"/>
+      <c r="W6" s="175"/>
+      <c r="X6" s="176"/>
     </row>
     <row r="7" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="13"/>
@@ -4115,18 +4117,18 @@
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
-      <c r="G8" s="159">
+      <c r="G8" s="165">
         <f>AVERAGE(G43:G50)*5</f>
         <v>0</v>
       </c>
-      <c r="H8" s="160"/>
-      <c r="I8" s="161"/>
-      <c r="V8" s="159">
+      <c r="H8" s="166"/>
+      <c r="I8" s="167"/>
+      <c r="V8" s="165">
         <f>AVERAGE(K43:K50)*5</f>
         <v>0</v>
       </c>
-      <c r="W8" s="160"/>
-      <c r="X8" s="161"/>
+      <c r="W8" s="166"/>
+      <c r="X8" s="167"/>
     </row>
     <row r="9" spans="2:24" ht="91" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="21"/>
@@ -4134,12 +4136,12 @@
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
-      <c r="G9" s="162"/>
-      <c r="H9" s="163"/>
-      <c r="I9" s="164"/>
-      <c r="V9" s="162"/>
-      <c r="W9" s="163"/>
-      <c r="X9" s="164"/>
+      <c r="G9" s="168"/>
+      <c r="H9" s="169"/>
+      <c r="I9" s="170"/>
+      <c r="V9" s="168"/>
+      <c r="W9" s="169"/>
+      <c r="X9" s="170"/>
     </row>
     <row r="10" spans="2:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="13"/>
@@ -4147,12 +4149,12 @@
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="162"/>
-      <c r="H10" s="163"/>
-      <c r="I10" s="164"/>
-      <c r="V10" s="162"/>
-      <c r="W10" s="163"/>
-      <c r="X10" s="164"/>
+      <c r="G10" s="168"/>
+      <c r="H10" s="169"/>
+      <c r="I10" s="170"/>
+      <c r="V10" s="168"/>
+      <c r="W10" s="169"/>
+      <c r="X10" s="170"/>
     </row>
     <row r="11" spans="2:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="13"/>
@@ -4160,19 +4162,19 @@
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="165"/>
-      <c r="H11" s="166"/>
-      <c r="I11" s="167"/>
-      <c r="V11" s="165"/>
-      <c r="W11" s="166"/>
-      <c r="X11" s="167"/>
+      <c r="G11" s="171"/>
+      <c r="H11" s="172"/>
+      <c r="I11" s="173"/>
+      <c r="V11" s="171"/>
+      <c r="W11" s="172"/>
+      <c r="X11" s="173"/>
     </row>
     <row r="12" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="171"/>
-      <c r="C12" s="171"/>
-      <c r="D12" s="171"/>
-      <c r="E12" s="171"/>
-      <c r="F12" s="171"/>
+      <c r="B12" s="160"/>
+      <c r="C12" s="160"/>
+      <c r="D12" s="160"/>
+      <c r="E12" s="160"/>
+      <c r="F12" s="160"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
@@ -4196,11 +4198,11 @@
       <c r="F15" s="13"/>
     </row>
     <row r="16" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="171"/>
-      <c r="C16" s="171"/>
-      <c r="D16" s="171"/>
-      <c r="E16" s="171"/>
-      <c r="F16" s="171"/>
+      <c r="B16" s="160"/>
+      <c r="C16" s="160"/>
+      <c r="D16" s="160"/>
+      <c r="E16" s="160"/>
+      <c r="F16" s="160"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="14"/>
@@ -4253,18 +4255,18 @@
     </row>
     <row r="35" spans="3:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="3:11" ht="14.5" x14ac:dyDescent="0.3">
-      <c r="D41" s="172" t="s">
+      <c r="D41" s="161" t="s">
         <v>115</v>
       </c>
-      <c r="E41" s="173"/>
-      <c r="F41" s="173"/>
-      <c r="G41" s="174"/>
-      <c r="H41" s="172" t="s">
+      <c r="E41" s="162"/>
+      <c r="F41" s="162"/>
+      <c r="G41" s="163"/>
+      <c r="H41" s="161" t="s">
         <v>116</v>
       </c>
-      <c r="I41" s="173"/>
-      <c r="J41" s="173"/>
-      <c r="K41" s="174"/>
+      <c r="I41" s="162"/>
+      <c r="J41" s="162"/>
+      <c r="K41" s="163"/>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.3">
       <c r="D42" s="17" t="s">
@@ -4590,6 +4592,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="V8:X11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="D41:G41"/>
@@ -4597,8 +4601,6 @@
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="G8:I11"/>
     <mergeCell ref="G6:I6"/>
-    <mergeCell ref="V6:X6"/>
-    <mergeCell ref="V8:X11"/>
   </mergeCells>
   <conditionalFormatting sqref="F14">
     <cfRule type="iconSet" priority="3">
@@ -4639,7 +4641,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:K85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView topLeftCell="B55" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
@@ -4659,16 +4661,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B1" s="175" t="s">
+      <c r="B1" s="177" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B2" s="73"/>
@@ -4696,10 +4698,10 @@
       <c r="F3" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="G3" s="176" t="s">
+      <c r="G3" s="178" t="s">
         <v>271</v>
       </c>
-      <c r="H3" s="176"/>
+      <c r="H3" s="178"/>
       <c r="I3" s="113" t="s">
         <v>108</v>
       </c>
@@ -5028,7 +5030,7 @@
       <c r="B20" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="179" t="s">
+      <c r="C20" s="131" t="s">
         <v>174</v>
       </c>
       <c r="D20" s="25" t="s">
@@ -5052,7 +5054,7 @@
       <c r="B21" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="179" t="s">
+      <c r="C21" s="131" t="s">
         <v>175</v>
       </c>
       <c r="D21" s="25" t="s">
@@ -5076,7 +5078,7 @@
       <c r="B22" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="179" t="s">
+      <c r="C22" s="131" t="s">
         <v>176</v>
       </c>
       <c r="D22" s="25" t="s">
@@ -5100,7 +5102,7 @@
       <c r="B23" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="179" t="s">
+      <c r="C23" s="131" t="s">
         <v>177</v>
       </c>
       <c r="D23" s="37"/>
@@ -5124,7 +5126,7 @@
       <c r="B24" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="179" t="s">
+      <c r="C24" s="131" t="s">
         <v>284</v>
       </c>
       <c r="D24" s="37"/>
@@ -5148,7 +5150,7 @@
       <c r="B25" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="179" t="s">
+      <c r="C25" s="131" t="s">
         <v>178</v>
       </c>
       <c r="D25" s="37"/>
@@ -5172,7 +5174,7 @@
       <c r="B26" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="179" t="s">
+      <c r="C26" s="131" t="s">
         <v>179</v>
       </c>
       <c r="D26" s="37"/>
@@ -5234,7 +5236,7 @@
       <c r="B29" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="179" t="s">
+      <c r="C29" s="131" t="s">
         <v>181</v>
       </c>
       <c r="D29" s="25" t="s">
@@ -5258,7 +5260,7 @@
       <c r="B30" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="179" t="s">
+      <c r="C30" s="131" t="s">
         <v>182</v>
       </c>
       <c r="D30" s="25" t="s">
@@ -5306,7 +5308,7 @@
       <c r="B32" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="179" t="s">
+      <c r="C32" s="131" t="s">
         <v>184</v>
       </c>
       <c r="D32" s="25" t="s">
@@ -5330,7 +5332,7 @@
       <c r="B33" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="179" t="s">
+      <c r="C33" s="131" t="s">
         <v>185</v>
       </c>
       <c r="D33" s="25" t="s">
@@ -5354,7 +5356,7 @@
       <c r="B34" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="179" t="s">
+      <c r="C34" s="131" t="s">
         <v>186</v>
       </c>
       <c r="D34" s="25" t="s">
@@ -5669,7 +5671,7 @@
       <c r="B48" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="C48" s="179" t="s">
+      <c r="C48" s="131" t="s">
         <v>198</v>
       </c>
       <c r="D48" s="25" t="s">
@@ -5827,7 +5829,7 @@
       <c r="B55" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="C55" s="179" t="s">
+      <c r="C55" s="131" t="s">
         <v>204</v>
       </c>
       <c r="D55" s="25" t="s">
@@ -5875,7 +5877,7 @@
       <c r="B57" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="C57" s="179" t="s">
+      <c r="C57" s="131" t="s">
         <v>206</v>
       </c>
       <c r="D57" s="25" t="s">
@@ -5899,7 +5901,7 @@
       <c r="B58" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="C58" s="179" t="s">
+      <c r="C58" s="131" t="s">
         <v>207</v>
       </c>
       <c r="D58" s="25" t="s">
@@ -5923,7 +5925,7 @@
       <c r="B59" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="C59" s="179" t="s">
+      <c r="C59" s="131" t="s">
         <v>208</v>
       </c>
       <c r="D59" s="25" t="s">
@@ -5995,7 +5997,7 @@
       <c r="B62" s="71" t="s">
         <v>224</v>
       </c>
-      <c r="C62" s="179" t="s">
+      <c r="C62" s="131" t="s">
         <v>210</v>
       </c>
       <c r="D62" s="25" t="s">
@@ -6033,7 +6035,7 @@
       <c r="B64" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="C64" s="179" t="s">
+      <c r="C64" s="131" t="s">
         <v>211</v>
       </c>
       <c r="D64" s="25" t="s">
@@ -6057,7 +6059,7 @@
       <c r="B65" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="C65" s="179" t="s">
+      <c r="C65" s="131" t="s">
         <v>212</v>
       </c>
       <c r="D65" s="25" t="s">
@@ -6081,7 +6083,7 @@
       <c r="B66" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="C66" s="179" t="s">
+      <c r="C66" s="131" t="s">
         <v>213</v>
       </c>
       <c r="D66" s="25" t="s">
@@ -6105,7 +6107,7 @@
       <c r="B67" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="C67" s="179" t="s">
+      <c r="C67" s="131" t="s">
         <v>214</v>
       </c>
       <c r="D67" s="25" t="s">
@@ -6153,7 +6155,7 @@
       <c r="B69" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="C69" s="179" t="s">
+      <c r="C69" s="131" t="s">
         <v>216</v>
       </c>
       <c r="D69" s="25" t="s">
@@ -6177,7 +6179,7 @@
       <c r="B70" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="C70" s="179" t="s">
+      <c r="C70" s="131" t="s">
         <v>217</v>
       </c>
       <c r="D70" s="25" t="s">
@@ -6201,7 +6203,7 @@
       <c r="B71" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="C71" s="179" t="s">
+      <c r="C71" s="131" t="s">
         <v>218</v>
       </c>
       <c r="D71" s="25" t="s">
@@ -6417,7 +6419,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B1:G29"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView topLeftCell="B8" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -6530,7 +6532,7 @@
       <c r="B7" s="70" t="s">
         <v>236</v>
       </c>
-      <c r="C7" s="179" t="s">
+      <c r="C7" s="131" t="s">
         <v>246</v>
       </c>
       <c r="D7" s="24" t="s">
@@ -6552,7 +6554,7 @@
       <c r="B8" s="70" t="s">
         <v>237</v>
       </c>
-      <c r="C8" s="179" t="s">
+      <c r="C8" s="131" t="s">
         <v>247</v>
       </c>
       <c r="D8" s="24" t="s">
@@ -6574,7 +6576,7 @@
       <c r="B9" s="70" t="s">
         <v>238</v>
       </c>
-      <c r="C9" s="179" t="s">
+      <c r="C9" s="131" t="s">
         <v>248</v>
       </c>
       <c r="D9" s="24" t="s">
@@ -6596,7 +6598,7 @@
       <c r="B10" s="70" t="s">
         <v>239</v>
       </c>
-      <c r="C10" s="179" t="s">
+      <c r="C10" s="131" t="s">
         <v>249</v>
       </c>
       <c r="D10" s="24" t="s">
@@ -6636,7 +6638,7 @@
       <c r="B12" s="70" t="s">
         <v>241</v>
       </c>
-      <c r="C12" s="179" t="s">
+      <c r="C12" s="131" t="s">
         <v>251</v>
       </c>
       <c r="D12" s="24" t="s">
@@ -6654,7 +6656,7 @@
       <c r="B13" s="70" t="s">
         <v>155</v>
       </c>
-      <c r="C13" s="179" t="s">
+      <c r="C13" s="131" t="s">
         <v>252</v>
       </c>
       <c r="D13" s="24" t="s">
@@ -6931,10 +6933,10 @@
       <c r="F3" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="G3" s="176" t="s">
+      <c r="G3" s="178" t="s">
         <v>271</v>
       </c>
-      <c r="H3" s="177"/>
+      <c r="H3" s="179"/>
       <c r="I3" s="113" t="s">
         <v>108</v>
       </c>
@@ -7263,7 +7265,7 @@
       <c r="B20" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="179" t="s">
+      <c r="C20" s="131" t="s">
         <v>174</v>
       </c>
       <c r="D20" s="25" t="s">
@@ -7287,7 +7289,7 @@
       <c r="B21" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="179" t="s">
+      <c r="C21" s="131" t="s">
         <v>175</v>
       </c>
       <c r="D21" s="25" t="s">
@@ -7311,7 +7313,7 @@
       <c r="B22" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="179" t="s">
+      <c r="C22" s="131" t="s">
         <v>176</v>
       </c>
       <c r="D22" s="25" t="s">
@@ -7335,7 +7337,7 @@
       <c r="B23" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="179" t="s">
+      <c r="C23" s="131" t="s">
         <v>177</v>
       </c>
       <c r="D23" s="37"/>
@@ -7359,7 +7361,7 @@
       <c r="B24" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="179" t="s">
+      <c r="C24" s="131" t="s">
         <v>284</v>
       </c>
       <c r="D24" s="37"/>
@@ -7383,7 +7385,7 @@
       <c r="B25" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="179" t="s">
+      <c r="C25" s="131" t="s">
         <v>178</v>
       </c>
       <c r="D25" s="37"/>
@@ -7407,7 +7409,7 @@
       <c r="B26" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="179" t="s">
+      <c r="C26" s="131" t="s">
         <v>179</v>
       </c>
       <c r="D26" s="37"/>
@@ -7471,7 +7473,7 @@
       <c r="B29" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="179" t="s">
+      <c r="C29" s="131" t="s">
         <v>181</v>
       </c>
       <c r="D29" s="25" t="s">
@@ -7495,7 +7497,7 @@
       <c r="B30" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="179" t="s">
+      <c r="C30" s="131" t="s">
         <v>182</v>
       </c>
       <c r="D30" s="25" t="s">
@@ -7543,7 +7545,7 @@
       <c r="B32" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="179" t="s">
+      <c r="C32" s="131" t="s">
         <v>184</v>
       </c>
       <c r="D32" s="25" t="s">
@@ -7567,7 +7569,7 @@
       <c r="B33" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="179" t="s">
+      <c r="C33" s="131" t="s">
         <v>185</v>
       </c>
       <c r="D33" s="25" t="s">
@@ -7591,7 +7593,7 @@
       <c r="B34" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="179" t="s">
+      <c r="C34" s="131" t="s">
         <v>186</v>
       </c>
       <c r="D34" s="25" t="s">
@@ -7906,7 +7908,7 @@
       <c r="B48" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="C48" s="179" t="s">
+      <c r="C48" s="131" t="s">
         <v>198</v>
       </c>
       <c r="D48" s="25" t="s">
@@ -8076,7 +8078,7 @@
       <c r="B55" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="C55" s="179" t="s">
+      <c r="C55" s="131" t="s">
         <v>204</v>
       </c>
       <c r="D55" s="25" t="s">
@@ -8124,7 +8126,7 @@
       <c r="B57" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="C57" s="179" t="s">
+      <c r="C57" s="131" t="s">
         <v>206</v>
       </c>
       <c r="D57" s="25" t="s">
@@ -8148,7 +8150,7 @@
       <c r="B58" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="C58" s="179" t="s">
+      <c r="C58" s="131" t="s">
         <v>207</v>
       </c>
       <c r="D58" s="25" t="s">
@@ -8172,7 +8174,7 @@
       <c r="B59" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="C59" s="179" t="s">
+      <c r="C59" s="131" t="s">
         <v>208</v>
       </c>
       <c r="D59" s="25" t="s">
@@ -8244,7 +8246,7 @@
       <c r="B62" s="68" t="s">
         <v>224</v>
       </c>
-      <c r="C62" s="179" t="s">
+      <c r="C62" s="131" t="s">
         <v>210</v>
       </c>
       <c r="D62" s="25" t="s">
@@ -8282,7 +8284,7 @@
       <c r="B64" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="C64" s="179" t="s">
+      <c r="C64" s="131" t="s">
         <v>211</v>
       </c>
       <c r="D64" s="25" t="s">
@@ -8306,7 +8308,7 @@
       <c r="B65" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="C65" s="179" t="s">
+      <c r="C65" s="131" t="s">
         <v>212</v>
       </c>
       <c r="D65" s="25" t="s">
@@ -8330,7 +8332,7 @@
       <c r="B66" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="C66" s="179" t="s">
+      <c r="C66" s="131" t="s">
         <v>213</v>
       </c>
       <c r="D66" s="25" t="s">
@@ -8354,7 +8356,7 @@
       <c r="B67" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="C67" s="179" t="s">
+      <c r="C67" s="131" t="s">
         <v>214</v>
       </c>
       <c r="D67" s="25" t="s">
@@ -8402,7 +8404,7 @@
       <c r="B69" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="C69" s="179" t="s">
+      <c r="C69" s="131" t="s">
         <v>216</v>
       </c>
       <c r="D69" s="25" t="s">
@@ -8426,7 +8428,7 @@
       <c r="B70" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="C70" s="179" t="s">
+      <c r="C70" s="131" t="s">
         <v>217</v>
       </c>
       <c r="D70" s="25" t="s">
@@ -8450,7 +8452,7 @@
       <c r="B71" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="C71" s="179" t="s">
+      <c r="C71" s="131" t="s">
         <v>218</v>
       </c>
       <c r="D71" s="25" t="s">
@@ -8776,7 +8778,7 @@
       <c r="B7" s="70" t="s">
         <v>236</v>
       </c>
-      <c r="C7" s="179" t="s">
+      <c r="C7" s="131" t="s">
         <v>246</v>
       </c>
       <c r="D7" s="24" t="s">
@@ -8798,7 +8800,7 @@
       <c r="B8" s="70" t="s">
         <v>237</v>
       </c>
-      <c r="C8" s="179" t="s">
+      <c r="C8" s="131" t="s">
         <v>247</v>
       </c>
       <c r="D8" s="24" t="s">
@@ -8816,7 +8818,7 @@
       <c r="B9" s="70" t="s">
         <v>238</v>
       </c>
-      <c r="C9" s="179" t="s">
+      <c r="C9" s="131" t="s">
         <v>248</v>
       </c>
       <c r="D9" s="24" t="s">
@@ -8834,7 +8836,7 @@
       <c r="B10" s="70" t="s">
         <v>239</v>
       </c>
-      <c r="C10" s="179" t="s">
+      <c r="C10" s="131" t="s">
         <v>249</v>
       </c>
       <c r="D10" s="24" t="s">
@@ -8870,7 +8872,7 @@
       <c r="B12" s="70" t="s">
         <v>241</v>
       </c>
-      <c r="C12" s="179" t="s">
+      <c r="C12" s="131" t="s">
         <v>251</v>
       </c>
       <c r="D12" s="24" t="s">
@@ -8888,7 +8890,7 @@
       <c r="B13" s="70" t="s">
         <v>155</v>
       </c>
-      <c r="C13" s="179" t="s">
+      <c r="C13" s="131" t="s">
         <v>252</v>
       </c>
       <c r="D13" s="24" t="s">
@@ -9163,8 +9165,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -9175,10 +9177,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="178" t="s">
+      <c r="A1" s="180" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="178"/>
+      <c r="B1" s="180"/>
       <c r="C1" s="51"/>
       <c r="D1" s="33"/>
       <c r="E1" s="33"/>
@@ -9489,7 +9491,7 @@
       <c r="B21" s="87" t="s">
         <v>283</v>
       </c>
-      <c r="C21" s="180" t="s">
+      <c r="C21" s="132" t="s">
         <v>279</v>
       </c>
       <c r="D21" s="43">
@@ -9499,18 +9501,18 @@
         <v>281</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A22" s="52" t="s">
         <v>259</v>
       </c>
       <c r="B22" s="87" t="s">
         <v>285</v>
       </c>
-      <c r="C22" s="180" t="s">
+      <c r="C22" s="132" t="s">
         <v>279</v>
       </c>
       <c r="D22" s="43">
-        <v>43645</v>
+        <v>43649</v>
       </c>
       <c r="E22" s="92" t="s">
         <v>286</v>

</xml_diff>

<commit_message>
Final Update for the French and English Excel files based on OSS19 restruction
</commit_message>
<xml_diff>
--- a/Checklists/Mobile_App_Security_Checklist-English_1.1.xlsx
+++ b/Checklists/Mobile_App_Security_Checklist-English_1.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abderrahmane.LAPTOP-NBPOQCF6\Personal\R&amp;D\OWASP\MSTG\owasp-mstg\Checklists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606517CC-7B3F-4EA8-B83A-2500B9593DC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5B7607-FADD-4887-BEEF-43F889A58E72}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="288">
   <si>
     <t>ID</t>
   </si>
@@ -1054,6 +1054,9 @@
     <t>Synchronizing the requirements wording in excel with the MASVS
 changes:
 2.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updating the link 2.12 for IOS </t>
   </si>
 </sst>
 </file>
@@ -2261,18 +2264,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2309,6 +2300,18 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -4074,11 +4077,11 @@
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="2:24" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="164"/>
-      <c r="C4" s="164"/>
-      <c r="D4" s="164"/>
-      <c r="E4" s="164"/>
-      <c r="F4" s="164"/>
+      <c r="B4" s="160"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="160"/>
+      <c r="E4" s="160"/>
+      <c r="F4" s="160"/>
     </row>
     <row r="5" spans="2:24" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="20"/>
@@ -4093,16 +4096,16 @@
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
-      <c r="G6" s="174" t="s">
+      <c r="G6" s="170" t="s">
         <v>117</v>
       </c>
-      <c r="H6" s="175"/>
-      <c r="I6" s="176"/>
-      <c r="V6" s="174" t="s">
+      <c r="H6" s="171"/>
+      <c r="I6" s="172"/>
+      <c r="V6" s="170" t="s">
         <v>117</v>
       </c>
-      <c r="W6" s="175"/>
-      <c r="X6" s="176"/>
+      <c r="W6" s="171"/>
+      <c r="X6" s="172"/>
     </row>
     <row r="7" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="13"/>
@@ -4117,18 +4120,18 @@
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
-      <c r="G8" s="165">
+      <c r="G8" s="161">
         <f>AVERAGE(G43:G50)*5</f>
         <v>0</v>
       </c>
-      <c r="H8" s="166"/>
-      <c r="I8" s="167"/>
-      <c r="V8" s="165">
+      <c r="H8" s="162"/>
+      <c r="I8" s="163"/>
+      <c r="V8" s="161">
         <f>AVERAGE(K43:K50)*5</f>
         <v>0</v>
       </c>
-      <c r="W8" s="166"/>
-      <c r="X8" s="167"/>
+      <c r="W8" s="162"/>
+      <c r="X8" s="163"/>
     </row>
     <row r="9" spans="2:24" ht="91" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="21"/>
@@ -4136,12 +4139,12 @@
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
-      <c r="G9" s="168"/>
-      <c r="H9" s="169"/>
-      <c r="I9" s="170"/>
-      <c r="V9" s="168"/>
-      <c r="W9" s="169"/>
-      <c r="X9" s="170"/>
+      <c r="G9" s="164"/>
+      <c r="H9" s="165"/>
+      <c r="I9" s="166"/>
+      <c r="V9" s="164"/>
+      <c r="W9" s="165"/>
+      <c r="X9" s="166"/>
     </row>
     <row r="10" spans="2:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="13"/>
@@ -4149,12 +4152,12 @@
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="168"/>
-      <c r="H10" s="169"/>
-      <c r="I10" s="170"/>
-      <c r="V10" s="168"/>
-      <c r="W10" s="169"/>
-      <c r="X10" s="170"/>
+      <c r="G10" s="164"/>
+      <c r="H10" s="165"/>
+      <c r="I10" s="166"/>
+      <c r="V10" s="164"/>
+      <c r="W10" s="165"/>
+      <c r="X10" s="166"/>
     </row>
     <row r="11" spans="2:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="13"/>
@@ -4162,19 +4165,19 @@
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="171"/>
-      <c r="H11" s="172"/>
-      <c r="I11" s="173"/>
-      <c r="V11" s="171"/>
-      <c r="W11" s="172"/>
-      <c r="X11" s="173"/>
+      <c r="G11" s="167"/>
+      <c r="H11" s="168"/>
+      <c r="I11" s="169"/>
+      <c r="V11" s="167"/>
+      <c r="W11" s="168"/>
+      <c r="X11" s="169"/>
     </row>
     <row r="12" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="160"/>
-      <c r="C12" s="160"/>
-      <c r="D12" s="160"/>
-      <c r="E12" s="160"/>
-      <c r="F12" s="160"/>
+      <c r="B12" s="173"/>
+      <c r="C12" s="173"/>
+      <c r="D12" s="173"/>
+      <c r="E12" s="173"/>
+      <c r="F12" s="173"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
@@ -4198,11 +4201,11 @@
       <c r="F15" s="13"/>
     </row>
     <row r="16" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="160"/>
-      <c r="C16" s="160"/>
-      <c r="D16" s="160"/>
-      <c r="E16" s="160"/>
-      <c r="F16" s="160"/>
+      <c r="B16" s="173"/>
+      <c r="C16" s="173"/>
+      <c r="D16" s="173"/>
+      <c r="E16" s="173"/>
+      <c r="F16" s="173"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="14"/>
@@ -4255,18 +4258,18 @@
     </row>
     <row r="35" spans="3:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="3:11" ht="14.5" x14ac:dyDescent="0.3">
-      <c r="D41" s="161" t="s">
+      <c r="D41" s="174" t="s">
         <v>115</v>
       </c>
-      <c r="E41" s="162"/>
-      <c r="F41" s="162"/>
-      <c r="G41" s="163"/>
-      <c r="H41" s="161" t="s">
+      <c r="E41" s="175"/>
+      <c r="F41" s="175"/>
+      <c r="G41" s="176"/>
+      <c r="H41" s="174" t="s">
         <v>116</v>
       </c>
-      <c r="I41" s="162"/>
-      <c r="J41" s="162"/>
-      <c r="K41" s="163"/>
+      <c r="I41" s="175"/>
+      <c r="J41" s="175"/>
+      <c r="K41" s="176"/>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.3">
       <c r="D42" s="17" t="s">
@@ -4592,8 +4595,6 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="V6:X6"/>
-    <mergeCell ref="V8:X11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="D41:G41"/>
@@ -4601,6 +4602,8 @@
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="G8:I11"/>
     <mergeCell ref="G6:I6"/>
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="V8:X11"/>
   </mergeCells>
   <conditionalFormatting sqref="F14">
     <cfRule type="iconSet" priority="3">
@@ -4641,8 +4644,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:K85"/>
   <sheetViews>
-    <sheetView topLeftCell="B55" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView topLeftCell="B21" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -6878,8 +6881,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:K85"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" zoomScale="74" zoomScaleNormal="74" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView topLeftCell="A16" zoomScale="74" zoomScaleNormal="74" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -7447,9 +7450,9 @@
       <c r="G27" s="125" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
-"0x06f-Testing-Local-Authentication.md#local-authentication-on-ios"),
-"Testing Local Authentication")</f>
-        <v>Testing Local Authentication</v>
+"0x04i-Testing-user-interaction.md#testing-user-education"),
+"Testing user education")</f>
+        <v>Testing user education</v>
       </c>
       <c r="H27" s="110"/>
       <c r="I27" s="115"/>
@@ -9163,10 +9166,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -9518,6 +9521,23 @@
         <v>286</v>
       </c>
     </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="52" t="s">
+        <v>259</v>
+      </c>
+      <c r="B23" s="87" t="s">
+        <v>285</v>
+      </c>
+      <c r="C23" s="132" t="s">
+        <v>279</v>
+      </c>
+      <c r="D23" s="43">
+        <v>43672</v>
+      </c>
+      <c r="E23" s="92" t="s">
+        <v>287</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Ensure that tiles are in sync on Excel and MSTG #1388
</commit_message>
<xml_diff>
--- a/Checklists/Mobile_App_Security_Checklist-English_1.1.xlsx
+++ b/Checklists/Mobile_App_Security_Checklist-English_1.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abderrahmane.LAPTOP-NBPOQCF6\Personal\R&amp;D\OWASP\MSTG\owasp-mstg\Checklists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5B7607-FADD-4887-BEEF-43F889A58E72}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AB9F59-A106-4ABC-ACAF-F77A669F022F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="289">
   <si>
     <t>ID</t>
   </si>
@@ -1057,6 +1057,9 @@
   </si>
   <si>
     <t xml:space="preserve">Updating the link 2.12 for IOS </t>
+  </si>
+  <si>
+    <t>Ensure that tiles are in sync on Excel and MSTG</t>
   </si>
 </sst>
 </file>
@@ -2184,13 +2187,34 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2225,12 +2249,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -2249,20 +2267,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2300,18 +2315,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -3652,48 +3655,48 @@
   <sheetData>
     <row r="1" spans="2:4" ht="8" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="144" t="s">
         <v>219</v>
       </c>
-      <c r="C2" s="138"/>
-      <c r="D2" s="139"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="146"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B3" s="140"/>
-      <c r="C3" s="141"/>
-      <c r="D3" s="142"/>
+      <c r="B3" s="147"/>
+      <c r="C3" s="148"/>
+      <c r="D3" s="149"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="140"/>
-      <c r="C4" s="141"/>
-      <c r="D4" s="142"/>
+      <c r="B4" s="147"/>
+      <c r="C4" s="148"/>
+      <c r="D4" s="149"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="140"/>
-      <c r="C5" s="141"/>
-      <c r="D5" s="142"/>
+      <c r="B5" s="147"/>
+      <c r="C5" s="148"/>
+      <c r="D5" s="149"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B6" s="140"/>
-      <c r="C6" s="141"/>
-      <c r="D6" s="142"/>
+      <c r="B6" s="147"/>
+      <c r="C6" s="148"/>
+      <c r="D6" s="149"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B7" s="140"/>
-      <c r="C7" s="141"/>
-      <c r="D7" s="142"/>
+      <c r="B7" s="147"/>
+      <c r="C7" s="148"/>
+      <c r="D7" s="149"/>
     </row>
     <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="143"/>
-      <c r="C8" s="144"/>
-      <c r="D8" s="145"/>
+      <c r="B8" s="150"/>
+      <c r="C8" s="151"/>
+      <c r="D8" s="152"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B9" s="146" t="s">
+      <c r="B9" s="153" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="147"/>
-      <c r="D9" s="148"/>
+      <c r="C9" s="140"/>
+      <c r="D9" s="141"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="126" t="s">
@@ -3703,19 +3706,19 @@
       <c r="D10" s="128"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B11" s="154" t="s">
+      <c r="B11" s="159" t="s">
         <v>278</v>
       </c>
-      <c r="C11" s="154"/>
+      <c r="C11" s="159"/>
       <c r="D11" s="129" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B12" s="135" t="s">
+      <c r="B12" s="133" t="s">
         <v>280</v>
       </c>
-      <c r="C12" s="136"/>
+      <c r="C12" s="143"/>
       <c r="D12" s="130" t="str">
         <f>HYPERLINK(CONCATENATE(
 "https://github.com/OWASP/owasp-masvs/blob/",
@@ -3725,19 +3728,19 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B13" s="149" t="s">
+      <c r="B13" s="154" t="s">
         <v>277</v>
       </c>
-      <c r="C13" s="150"/>
+      <c r="C13" s="155"/>
       <c r="D13" s="12" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B14" s="135" t="s">
+      <c r="B14" s="133" t="s">
         <v>221</v>
       </c>
-      <c r="C14" s="136"/>
+      <c r="C14" s="143"/>
       <c r="D14" s="124" t="str">
         <f>HYPERLINK(CONCATENATE(
 "https://github.com/OWASP/owasp-mstg/blob/",
@@ -3747,69 +3750,69 @@
       </c>
     </row>
     <row r="15" spans="2:4" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="151" t="s">
+      <c r="B15" s="156" t="s">
         <v>263</v>
       </c>
-      <c r="C15" s="152"/>
-      <c r="D15" s="153"/>
+      <c r="C15" s="157"/>
+      <c r="D15" s="158"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B16" s="133" t="s">
+      <c r="B16" s="138" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="134"/>
+      <c r="C16" s="139"/>
       <c r="D16" s="12"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="135" t="s">
+      <c r="B17" s="133" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="136"/>
+      <c r="C17" s="143"/>
       <c r="D17" s="12"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="133" t="s">
+      <c r="B18" s="138" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="134"/>
+      <c r="C18" s="139"/>
       <c r="D18" s="12"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="133" t="s">
+      <c r="B19" s="138" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="134"/>
+      <c r="C19" s="139"/>
       <c r="D19" s="12"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="133" t="s">
+      <c r="B20" s="138" t="s">
         <v>135</v>
       </c>
-      <c r="C20" s="134"/>
+      <c r="C20" s="139"/>
       <c r="D20" s="12"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="133" t="s">
+      <c r="B21" s="138" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="134"/>
+      <c r="C21" s="139"/>
       <c r="D21" s="12" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="133" t="s">
+      <c r="B22" s="138" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="134"/>
+      <c r="C22" s="139"/>
       <c r="D22" s="12" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B23" s="147"/>
-      <c r="C23" s="147"/>
-      <c r="D23" s="148"/>
+      <c r="B23" s="140"/>
+      <c r="C23" s="140"/>
+      <c r="D23" s="141"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
@@ -3826,37 +3829,37 @@
       <c r="D25" s="12"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B26" s="133" t="s">
+      <c r="B26" s="138" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="134"/>
+      <c r="C26" s="139"/>
       <c r="D26" s="12"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B27" s="133" t="s">
+      <c r="B27" s="138" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="134"/>
+      <c r="C27" s="139"/>
       <c r="D27" s="12"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B28" s="133" t="s">
+      <c r="B28" s="138" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="134"/>
+      <c r="C28" s="139"/>
       <c r="D28" s="12"/>
     </row>
     <row r="29" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="159" t="s">
+      <c r="B29" s="142" t="s">
         <v>257</v>
       </c>
-      <c r="C29" s="134"/>
+      <c r="C29" s="139"/>
       <c r="D29" s="12"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B30" s="147"/>
-      <c r="C30" s="147"/>
-      <c r="D30" s="148"/>
+      <c r="B30" s="140"/>
+      <c r="C30" s="140"/>
+      <c r="D30" s="141"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
@@ -3873,37 +3876,37 @@
       <c r="D32" s="12"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B33" s="133" t="s">
+      <c r="B33" s="138" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="134"/>
+      <c r="C33" s="139"/>
       <c r="D33" s="12"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B34" s="133" t="s">
+      <c r="B34" s="138" t="s">
         <v>99</v>
       </c>
-      <c r="C34" s="134"/>
+      <c r="C34" s="139"/>
       <c r="D34" s="12"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B35" s="133" t="s">
+      <c r="B35" s="138" t="s">
         <v>100</v>
       </c>
-      <c r="C35" s="134"/>
+      <c r="C35" s="139"/>
       <c r="D35" s="12"/>
     </row>
     <row r="36" spans="2:4" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="159" t="s">
+      <c r="B36" s="142" t="s">
         <v>258</v>
       </c>
-      <c r="C36" s="134"/>
+      <c r="C36" s="139"/>
       <c r="D36" s="12"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B37" s="147"/>
-      <c r="C37" s="147"/>
-      <c r="D37" s="148"/>
+      <c r="B37" s="140"/>
+      <c r="C37" s="140"/>
+      <c r="D37" s="141"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
@@ -3913,97 +3916,100 @@
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B39" s="155"/>
-      <c r="C39" s="156"/>
-      <c r="D39" s="157"/>
+      <c r="B39" s="135"/>
+      <c r="C39" s="136"/>
+      <c r="D39" s="137"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B40" s="135" t="s">
+      <c r="B40" s="133" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="158"/>
+      <c r="C40" s="134"/>
       <c r="D40" s="39"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B41" s="135" t="s">
+      <c r="B41" s="133" t="s">
         <v>92</v>
       </c>
-      <c r="C41" s="158"/>
+      <c r="C41" s="134"/>
       <c r="D41" s="39"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B42" s="135" t="s">
+      <c r="B42" s="133" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="158"/>
+      <c r="C42" s="134"/>
       <c r="D42" s="39"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B43" s="135" t="s">
+      <c r="B43" s="133" t="s">
         <v>94</v>
       </c>
-      <c r="C43" s="158"/>
+      <c r="C43" s="134"/>
       <c r="D43" s="40"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B44" s="135" t="s">
+      <c r="B44" s="133" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="158"/>
+      <c r="C44" s="134"/>
       <c r="D44" s="39"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B45" s="155"/>
-      <c r="C45" s="156"/>
-      <c r="D45" s="157"/>
+      <c r="B45" s="135"/>
+      <c r="C45" s="136"/>
+      <c r="D45" s="137"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B46" s="135" t="s">
+      <c r="B46" s="133" t="s">
         <v>91</v>
       </c>
-      <c r="C46" s="158"/>
+      <c r="C46" s="134"/>
       <c r="D46" s="39"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B47" s="135" t="s">
+      <c r="B47" s="133" t="s">
         <v>92</v>
       </c>
-      <c r="C47" s="158"/>
+      <c r="C47" s="134"/>
       <c r="D47" s="39"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B48" s="135" t="s">
+      <c r="B48" s="133" t="s">
         <v>93</v>
       </c>
-      <c r="C48" s="158"/>
+      <c r="C48" s="134"/>
       <c r="D48" s="39"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B49" s="135" t="s">
+      <c r="B49" s="133" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="158"/>
+      <c r="C49" s="134"/>
       <c r="D49" s="40"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B50" s="135" t="s">
+      <c r="B50" s="133" t="s">
         <v>95</v>
       </c>
-      <c r="C50" s="158"/>
+      <c r="C50" s="134"/>
       <c r="D50" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B2:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B39:D39"/>
@@ -4018,19 +4024,16 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B2:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:C46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4077,11 +4080,11 @@
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="2:24" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="160"/>
-      <c r="C4" s="160"/>
-      <c r="D4" s="160"/>
-      <c r="E4" s="160"/>
-      <c r="F4" s="160"/>
+      <c r="B4" s="164"/>
+      <c r="C4" s="164"/>
+      <c r="D4" s="164"/>
+      <c r="E4" s="164"/>
+      <c r="F4" s="164"/>
     </row>
     <row r="5" spans="2:24" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="20"/>
@@ -4096,16 +4099,16 @@
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
-      <c r="G6" s="170" t="s">
+      <c r="G6" s="174" t="s">
         <v>117</v>
       </c>
-      <c r="H6" s="171"/>
-      <c r="I6" s="172"/>
-      <c r="V6" s="170" t="s">
+      <c r="H6" s="175"/>
+      <c r="I6" s="176"/>
+      <c r="V6" s="174" t="s">
         <v>117</v>
       </c>
-      <c r="W6" s="171"/>
-      <c r="X6" s="172"/>
+      <c r="W6" s="175"/>
+      <c r="X6" s="176"/>
     </row>
     <row r="7" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="13"/>
@@ -4120,18 +4123,18 @@
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
-      <c r="G8" s="161">
+      <c r="G8" s="165">
         <f>AVERAGE(G43:G50)*5</f>
         <v>0</v>
       </c>
-      <c r="H8" s="162"/>
-      <c r="I8" s="163"/>
-      <c r="V8" s="161">
+      <c r="H8" s="166"/>
+      <c r="I8" s="167"/>
+      <c r="V8" s="165">
         <f>AVERAGE(K43:K50)*5</f>
         <v>0</v>
       </c>
-      <c r="W8" s="162"/>
-      <c r="X8" s="163"/>
+      <c r="W8" s="166"/>
+      <c r="X8" s="167"/>
     </row>
     <row r="9" spans="2:24" ht="91" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="21"/>
@@ -4139,12 +4142,12 @@
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
-      <c r="G9" s="164"/>
-      <c r="H9" s="165"/>
-      <c r="I9" s="166"/>
-      <c r="V9" s="164"/>
-      <c r="W9" s="165"/>
-      <c r="X9" s="166"/>
+      <c r="G9" s="168"/>
+      <c r="H9" s="169"/>
+      <c r="I9" s="170"/>
+      <c r="V9" s="168"/>
+      <c r="W9" s="169"/>
+      <c r="X9" s="170"/>
     </row>
     <row r="10" spans="2:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="13"/>
@@ -4152,12 +4155,12 @@
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="164"/>
-      <c r="H10" s="165"/>
-      <c r="I10" s="166"/>
-      <c r="V10" s="164"/>
-      <c r="W10" s="165"/>
-      <c r="X10" s="166"/>
+      <c r="G10" s="168"/>
+      <c r="H10" s="169"/>
+      <c r="I10" s="170"/>
+      <c r="V10" s="168"/>
+      <c r="W10" s="169"/>
+      <c r="X10" s="170"/>
     </row>
     <row r="11" spans="2:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="13"/>
@@ -4165,19 +4168,19 @@
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="167"/>
-      <c r="H11" s="168"/>
-      <c r="I11" s="169"/>
-      <c r="V11" s="167"/>
-      <c r="W11" s="168"/>
-      <c r="X11" s="169"/>
+      <c r="G11" s="171"/>
+      <c r="H11" s="172"/>
+      <c r="I11" s="173"/>
+      <c r="V11" s="171"/>
+      <c r="W11" s="172"/>
+      <c r="X11" s="173"/>
     </row>
     <row r="12" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="173"/>
-      <c r="C12" s="173"/>
-      <c r="D12" s="173"/>
-      <c r="E12" s="173"/>
-      <c r="F12" s="173"/>
+      <c r="B12" s="160"/>
+      <c r="C12" s="160"/>
+      <c r="D12" s="160"/>
+      <c r="E12" s="160"/>
+      <c r="F12" s="160"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
@@ -4201,11 +4204,11 @@
       <c r="F15" s="13"/>
     </row>
     <row r="16" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="173"/>
-      <c r="C16" s="173"/>
-      <c r="D16" s="173"/>
-      <c r="E16" s="173"/>
-      <c r="F16" s="173"/>
+      <c r="B16" s="160"/>
+      <c r="C16" s="160"/>
+      <c r="D16" s="160"/>
+      <c r="E16" s="160"/>
+      <c r="F16" s="160"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="14"/>
@@ -4258,18 +4261,18 @@
     </row>
     <row r="35" spans="3:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="3:11" ht="14.5" x14ac:dyDescent="0.3">
-      <c r="D41" s="174" t="s">
+      <c r="D41" s="161" t="s">
         <v>115</v>
       </c>
-      <c r="E41" s="175"/>
-      <c r="F41" s="175"/>
-      <c r="G41" s="176"/>
-      <c r="H41" s="174" t="s">
+      <c r="E41" s="162"/>
+      <c r="F41" s="162"/>
+      <c r="G41" s="163"/>
+      <c r="H41" s="161" t="s">
         <v>116</v>
       </c>
-      <c r="I41" s="175"/>
-      <c r="J41" s="175"/>
-      <c r="K41" s="176"/>
+      <c r="I41" s="162"/>
+      <c r="J41" s="162"/>
+      <c r="K41" s="163"/>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.3">
       <c r="D42" s="17" t="s">
@@ -4595,6 +4598,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="V8:X11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="D41:G41"/>
@@ -4602,8 +4607,6 @@
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="G8:I11"/>
     <mergeCell ref="G6:I6"/>
-    <mergeCell ref="V6:X6"/>
-    <mergeCell ref="V8:X11"/>
   </mergeCells>
   <conditionalFormatting sqref="F14">
     <cfRule type="iconSet" priority="3">
@@ -4644,8 +4647,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:K85"/>
   <sheetViews>
-    <sheetView topLeftCell="B21" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView topLeftCell="B44" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -4955,8 +4958,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05d-Testing-Data-Storage.md#testing-local-storage-for-sensitive-data"),
-"Testing For Sensitive Data in Local Data Storage")</f>
-        <v>Testing For Sensitive Data in Local Data Storage</v>
+"Testing Local Storage for Sensitive Data")</f>
+        <v>Testing Local Storage for Sensitive Data</v>
       </c>
       <c r="H16" s="97"/>
       <c r="I16" s="115"/>
@@ -4975,8 +4978,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05d-Testing-Data-Storage.md#testing-local-storage-for-sensitive-data"),
-"Testing For Sensitive Data in Local Data Storage")</f>
-        <v>Testing For Sensitive Data in Local Data Storage</v>
+"Testing Local Storage for Sensitive Data")</f>
+        <v>Testing Local Storage for Sensitive Data</v>
       </c>
       <c r="H17" s="105"/>
       <c r="I17" s="119"/>
@@ -4999,8 +5002,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05d-Testing-Data-Storage.md#testing-logs-for-sensitive-data"),
-"Testing For Sensitive Data in Logs")</f>
-        <v>Testing For Sensitive Data in Logs</v>
+"Testing Logs for Sensitive Data")</f>
+        <v>Testing Logs for Sensitive Data</v>
       </c>
       <c r="H18" s="97"/>
       <c r="I18" s="115"/>
@@ -5023,8 +5026,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05d-Testing-Data-Storage.md#determining-whether-sensitive-data-is-sent-to-third-parties"),
-"Testing Whether Sensitive Data Is Sent To Third Parties")</f>
-        <v>Testing Whether Sensitive Data Is Sent To Third Parties</v>
+"Determining Whether Sensitive Data is Sent to Third Parties")</f>
+        <v>Determining Whether Sensitive Data is Sent to Third Parties</v>
       </c>
       <c r="H19" s="97"/>
       <c r="I19" s="115"/>
@@ -5047,8 +5050,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05d-Testing-Data-Storage.md#determining-whether-the-keyboard-cache-is-disabled-for-text-input-fields"),
-"Testing Whether the Keyboard Cache Is Disabled for Text Input Fields")</f>
-        <v>Testing Whether the Keyboard Cache Is Disabled for Text Input Fields</v>
+"Determining Whether the Keyboard Cache Is Disabled for Text Input Fields")</f>
+        <v>Determining Whether the Keyboard Cache Is Disabled for Text Input Fields</v>
       </c>
       <c r="H20" s="97"/>
       <c r="I20" s="115"/>
@@ -5071,8 +5074,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05d-Testing-Data-Storage.md#determining-whether-sensitive-stored-data-has-been-exposed-via-ipc-mechanisms"),
-"Testing Whether Sensitive Data Is Exposed via IPC Mechanisms")</f>
-        <v>Testing Whether Sensitive Data Is Exposed via IPC Mechanisms</v>
+"Determining Whether Sensitive Stored Data Has Been Exposed via IPC Mechanisms")</f>
+        <v>Determining Whether Sensitive Stored Data Has Been Exposed via IPC Mechanisms</v>
       </c>
       <c r="H21" s="97"/>
       <c r="I21" s="115"/>
@@ -5095,8 +5098,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05d-Testing-Data-Storage.md#checking-for-sensitive-data-disclosure-through-the-user-interface"),
-"Testing for Sensitive Data Disclosure Through the User Interface")</f>
-        <v>Testing for Sensitive Data Disclosure Through the User Interface</v>
+"Checking for Sensitive Data Disclosure Through the User Interface")</f>
+        <v>Checking for Sensitive Data Disclosure Through the User Interface</v>
       </c>
       <c r="H22" s="97"/>
       <c r="I22" s="115"/>
@@ -5119,8 +5122,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05d-Testing-Data-Storage.md#testing-backups-for-sensitive-data"),
-"Testing for Sensitive Data in Backups")</f>
-        <v>Testing for Sensitive Data in Backups</v>
+"Testing Backups for Sensitive Data")</f>
+        <v>Testing Backups for Sensitive Data</v>
       </c>
       <c r="H23" s="97"/>
       <c r="I23" s="115"/>
@@ -5143,8 +5146,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05d-Testing-Data-Storage.md#finding-sensitive-information-in-auto-generated-screenshots"),
-"Testing for Sensitive Information in Auto-Generated Screenshots")</f>
-        <v>Testing for Sensitive Information in Auto-Generated Screenshots</v>
+"Finding Sensitive Information in Auto-Generated Screenshots")</f>
+        <v>Finding Sensitive Information in Auto-Generated Screenshots</v>
       </c>
       <c r="H24" s="97"/>
       <c r="I24" s="115"/>
@@ -5167,8 +5170,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05d-Testing-Data-Storage.md#checking-memory-for-sensitive-data"),
-"Testing for Sensitive Data in Memory")</f>
-        <v>Testing for Sensitive Data in Memory</v>
+"Checking Memory for Sensitive Data")</f>
+        <v>Checking Memory for Sensitive Data</v>
       </c>
       <c r="H25" s="97"/>
       <c r="I25" s="115"/>
@@ -5215,8 +5218,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04i-Testing-user-interaction.md#testing-user-education"),
-"Testing user education")</f>
-        <v>Testing user education</v>
+"Testing User Education")</f>
+        <v>Testing User Education</v>
       </c>
       <c r="H27" s="97"/>
       <c r="I27" s="115"/>
@@ -5253,8 +5256,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05e-Testing-Cryptography.md#testing-key-management"),
-"Verifying Key Management")</f>
-        <v>Verifying Key Management</v>
+"Testing Key Management")</f>
+        <v>Testing Key Management</v>
       </c>
       <c r="H29" s="97"/>
       <c r="I29" s="115"/>
@@ -5277,8 +5280,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04g-Testing-Cryptography.md#cryptography-for-mobile-apps"),
-"Testing for Custom Implementations of Cryptography")</f>
-        <v>Testing for Custom Implementations of Cryptography</v>
+"Cryptography for Mobile Apps")</f>
+        <v>Cryptography for Mobile Apps</v>
       </c>
       <c r="H30" s="97"/>
       <c r="I30" s="115"/>
@@ -5325,8 +5328,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04g-Testing-Cryptography.md#identifying-insecure-andor-deprecated-cryptographic-algorithms"),
-"Testing for Insecure and/or Deprecated Cryptographic Algorithms")</f>
-        <v>Testing for Insecure and/or Deprecated Cryptographic Algorithms</v>
+"Identifying Insecure and/or Deprecated Cryptographic Algorithms")</f>
+        <v>Identifying Insecure and/or Deprecated Cryptographic Algorithms</v>
       </c>
       <c r="H32" s="97"/>
       <c r="I32" s="115"/>
@@ -5349,8 +5352,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05e-Testing-Cryptography.md#testing-key-management"),
-"Verifying Key Management")</f>
-        <v>Verifying Key Management</v>
+"Testing Key Management")</f>
+        <v>Testing Key Management</v>
       </c>
       <c r="H33" s="97"/>
       <c r="I33" s="115"/>
@@ -5411,8 +5414,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04e-Testing-Authentication-and-Session-Management.md#testing-authentication"),
-"Verifying that Users Are Properly Authenticated")</f>
-        <v>Verifying that Users Are Properly Authenticated</v>
+"Testing Authentication")</f>
+        <v>Testing Authentication</v>
       </c>
       <c r="H36" s="97"/>
       <c r="I36" s="115"/>
@@ -5459,8 +5462,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04e-Testing-Authentication-and-Session-Management.md#testing-stateless-token-based-authentication"),
-"Testing Stateless Authentication")</f>
-        <v>Testing Stateless Authentication</v>
+"Testing Stateless (Token-Based) Authentication")</f>
+        <v>Testing Stateless (Token-Based) Authentication</v>
       </c>
       <c r="H38" s="97"/>
       <c r="I38" s="115"/>
@@ -5480,8 +5483,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04e-Testing-Authentication-and-Session-Management.md#user-logout-and-session-timeouts"),
-"Testing the Logout Functionality")</f>
-        <v>Testing the Logout Functionality</v>
+"User Logout and Session Timeouts")</f>
+        <v>User Logout and Session Timeouts</v>
       </c>
       <c r="H39" s="97"/>
       <c r="I39" s="115"/>
@@ -5505,8 +5508,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04e-Testing-Authentication-and-Session-Management.md#best-practices-for-passwords"),
-"Testing the Password Policy")</f>
-        <v>Testing the Password Policy</v>
+"Best Practices for Passwords")</f>
+        <v>Best Practices for Passwords</v>
       </c>
       <c r="H40" s="97"/>
       <c r="I40" s="115"/>
@@ -5529,8 +5532,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04e-Testing-Authentication-and-Session-Management.md#running-a-password-dictionary-attack"),
-"Testing Excessive Login Attempts")</f>
-        <v>Testing Excessive Login Attempts</v>
+"Running a Password Dictionary Attack")</f>
+        <v>Running a Password Dictionary Attack</v>
       </c>
       <c r="H41" s="97"/>
       <c r="I41" s="115"/>
@@ -5553,8 +5556,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04e-Testing-Authentication-and-Session-Management.md#session-timeout"),
-"Testing the Session Timeout")</f>
-        <v>Testing the Session Timeout</v>
+"Session Timeout")</f>
+        <v>Session Timeout</v>
       </c>
       <c r="H42" s="97"/>
       <c r="I42" s="117"/>
@@ -5601,8 +5604,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-2fa-is-enforced"),
-"Testing 2-Factor Authentication")</f>
-        <v>Testing 2-Factor Authentication</v>
+"Verifying that 2FA is Enforced")</f>
+        <v>Verifying that 2FA is Enforced</v>
       </c>
       <c r="H44" s="97"/>
       <c r="I44" s="115"/>
@@ -5625,8 +5628,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04e-Testing-Authentication-and-Session-Management.md#2-factor-authentication-and-step-up-authentication"),
-"Testing Step-up Authentication")</f>
-        <v>Testing Step-up Authentication</v>
+"2-Factor Authentication and Step-up Authentication")</f>
+        <v>2-Factor Authentication and Step-up Authentication</v>
       </c>
       <c r="H45" s="97"/>
       <c r="I45" s="115"/>
@@ -5650,8 +5653,8 @@
 CONCATENATE(
 BASE_URL,
 "0x04e-Testing-Authentication-and-Session-Management.md#login-activity-and-device-blocking"),
-"Testing Login Activity and Device Blocking")</f>
-        <v>Testing Login Activity and Device Blocking</v>
+"Login Activity and Device Blocking")</f>
+        <v>Login Activity and Device Blocking</v>
       </c>
       <c r="H46" s="97"/>
       <c r="I46" s="115"/>
@@ -5688,8 +5691,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network"),
-"Testing for Unencrypted Sensitive Data on the Network")</f>
-        <v>Testing for Unencrypted Sensitive Data on the Network</v>
+"Verifying Data Encryption on the Network")</f>
+        <v>Verifying Data Encryption on the Network</v>
       </c>
       <c r="H48" s="97"/>
       <c r="I48" s="115"/>
@@ -5712,8 +5715,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04f-Testing-Network-Communication.md#recommended-tls-settings"),
-"Verifying the TLS Settings")</f>
-        <v>Verifying the TLS Settings</v>
+"Recommended TLS Settings")</f>
+        <v>Recommended TLS Settings</v>
       </c>
       <c r="H49" s="97"/>
       <c r="I49" s="115"/>
@@ -5760,8 +5763,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05g-Testing-Network-Communication.md#testing-custom-certificate-stores-and-certificate-pinning"),
-"Testing Custom Certificate Stores and SSL Pinning")</f>
-        <v>Testing Custom Certificate Stores and SSL Pinning</v>
+"Testing Custom Certificate Stores and Certificate Pinning")</f>
+        <v>Testing Custom Certificate Stores and Certificate Pinning</v>
       </c>
       <c r="H51" s="97"/>
       <c r="I51" s="115"/>
@@ -5784,8 +5787,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04f-Testing-Network-Communication.md#making-sure-that-critical-operations-use-secure-communication-channels"),
-"Verifying that Critical Operations Use Secure Communication Channels")</f>
-        <v>Verifying that Critical Operations Use Secure Communication Channels</v>
+"Making Sure that Critical Operations Use Secure Communication Channels")</f>
+        <v>Making Sure that Critical Operations Use Secure Communication Channels</v>
       </c>
       <c r="H52" s="97"/>
       <c r="I52" s="115"/>
@@ -5808,8 +5811,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05g-Testing-Network-Communication.md#testing-the-security-provider"),
-"Verifying the Security Provider")</f>
-        <v>Verifying the Security Provider</v>
+"Testing the Security Provider")</f>
+        <v>Testing the Security Provider</v>
       </c>
       <c r="H53" s="97"/>
       <c r="I53" s="115"/>
@@ -5870,8 +5873,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04h-Testing-Code-Quality.md#injection-flaws"),
-"Testing Input Validation and Sanitization")</f>
-        <v>Testing Input Validation and Sanitization</v>
+"Injection Flaws")</f>
+        <v>Injection Flaws</v>
       </c>
       <c r="H56" s="97"/>
       <c r="I56" s="115"/>
@@ -5918,8 +5921,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05h-Testing-Platform-Interaction.md#testing-for-sensitive-functionality-exposure-through-ipc"),
-"Testing For Sensitive Functionality Exposure Through IPC")</f>
-        <v>Testing For Sensitive Functionality Exposure Through IPC</v>
+"Testing for Sensitive Functionality Exposure Through IPC")</f>
+        <v>Testing for Sensitive Functionality Exposure Through IPC</v>
       </c>
       <c r="H58" s="97"/>
       <c r="I58" s="115"/>
@@ -5990,8 +5993,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05h-Testing-Platform-Interaction.md#determining-whether-java-objects-are-exposed-through-webviews"),
-"Testing Whether Java Objects Are Exposed Through WebViews")</f>
-        <v>Testing Whether Java Objects Are Exposed Through WebViews</v>
+"Determining Whether Java Objects Are Exposed Through WebViews")</f>
+        <v>Determining Whether Java Objects Are Exposed Through WebViews</v>
       </c>
       <c r="H61" s="97"/>
       <c r="I61" s="115"/>
@@ -6014,8 +6017,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05h-Testing-Platform-Interaction.md#testing-object-persistence"),
-"Testing Object (De-)Serialization")</f>
-        <v>Testing Object (De-)Serialization</v>
+"Testing Object Persistence")</f>
+        <v>Testing Object Persistence</v>
       </c>
       <c r="H62" s="97"/>
       <c r="I62" s="115"/>
@@ -6052,8 +6055,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05i-Testing-Code-Quality-and-Build-Settings.md#making-sure-that-the-app-is-properly-signed"),
-"Verifying That the App is Properly Signed")</f>
-        <v>Verifying That the App is Properly Signed</v>
+"Making Sure That the App is Properly Signed")</f>
+        <v>Making Sure That the App is Properly Signed</v>
       </c>
       <c r="H64" s="97"/>
       <c r="I64" s="115"/>
@@ -6076,8 +6079,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05i-Testing-Code-Quality-and-Build-Settings.md#determining-whether-the-app-is-debuggable"),
-"Testing If the App is Debuggable")</f>
-        <v>Testing If the App is Debuggable</v>
+"Determining Whether the App is Debuggable")</f>
+        <v>Determining Whether the App is Debuggable</v>
       </c>
       <c r="H65" s="97"/>
       <c r="I65" s="115"/>
@@ -6100,8 +6103,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05i-Testing-Code-Quality-and-Build-Settings.md#finding-debugging-symbols"),
-"Testing for Debugging Symbols")</f>
-        <v>Testing for Debugging Symbols</v>
+"Finding Debugging Symbols")</f>
+        <v>Finding Debugging Symbols</v>
       </c>
       <c r="H66" s="97"/>
       <c r="I66" s="115"/>
@@ -6124,8 +6127,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05i-Testing-Code-Quality-and-Build-Settings.md#finding-debugging-code-and-verbose-error-logging"),
-"Testing for Debugging Code and Verbose Error Logging")</f>
-        <v>Testing for Debugging Code and Verbose Error Logging</v>
+"Finding Debugging Code and Verbose Error Logging")</f>
+        <v>Finding Debugging Code and Verbose Error Logging</v>
       </c>
       <c r="H67" s="97"/>
       <c r="I67" s="115"/>
@@ -6148,8 +6151,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05i-Testing-Code-Quality-and-Build-Settings.md#checking-for-weaknesses-in-third-party-libraries"),
-"Testing for Weaknesses in Third Party Libraries")</f>
-        <v>Testing for Weaknesses in Third Party Libraries</v>
+"Checking for Weaknesses in Third Party Libraries")</f>
+        <v>Checking for Weaknesses in Third Party Libraries</v>
       </c>
       <c r="H68" s="98"/>
       <c r="I68" s="115"/>
@@ -6196,8 +6199,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling"),
-"Testing  Error Handling in Security Controls")</f>
-        <v>Testing  Error Handling in Security Controls</v>
+"Testing Exception Handling")</f>
+        <v>Testing Exception Handling</v>
       </c>
       <c r="H70" s="97"/>
       <c r="I70" s="115"/>
@@ -6220,8 +6223,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04h-Testing-Code-Quality.md#memory-corruption-bugs"),
-"Testing for Memory Management Bugs")</f>
-        <v>Testing for Memory Management Bugs</v>
+"Memory Corruption Bugs")</f>
+        <v>Memory Corruption Bugs</v>
       </c>
       <c r="H71" s="97"/>
       <c r="I71" s="121"/>
@@ -6245,8 +6248,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05i-Testing-Code-Quality-and-Build-Settings.md#make-sure-that-free-security-features-are-activated"),
-"Verifying usage of Free Security Features")</f>
-        <v>Verifying usage of Free Security Features</v>
+"Make Sure That Free Security Features Are Activated")</f>
+        <v>Make Sure That Free Security Features Are Activated</v>
       </c>
       <c r="H72" s="97"/>
       <c r="I72" s="115"/>
@@ -6422,8 +6425,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B1:G29"/>
   <sheetViews>
-    <sheetView topLeftCell="B8" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="C7" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -6526,8 +6529,8 @@
 CONCATENATE(
 BASE_URL,
 "0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-anti-debugging"),
-"Testing Debugging Defenses")</f>
-        <v>Testing Debugging Defenses</v>
+"Testing Anti-Debugging")</f>
+        <v>Testing Anti-Debugging</v>
       </c>
       <c r="G6" s="115"/>
     </row>
@@ -6570,8 +6573,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-the-detection-of-reverse-engineering-tools"),
-"Testing Detection of Reverse Engineering Tools")</f>
-        <v>Testing Detection of Reverse Engineering Tools</v>
+"Testing The Detection of Reverse Engineering Tools")</f>
+        <v>Testing The Detection of Reverse Engineering Tools</v>
       </c>
       <c r="G8" s="115"/>
     </row>
@@ -6592,8 +6595,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-emulator-detection"),
-"Testing Simple Emulator Detection")</f>
-        <v>Testing Simple Emulator Detection</v>
+"Testing Emulator Detection")</f>
+        <v>Testing Emulator Detection</v>
       </c>
       <c r="G9" s="115"/>
     </row>
@@ -6614,8 +6617,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-run-time-integrity-checks"),
-"Testing Run-Time Integrity Checks")</f>
-        <v>Testing Run-Time Integrity Checks</v>
+"Testing Run Time Integrity Checks")</f>
+        <v>Testing Run Time Integrity Checks</v>
       </c>
       <c r="G10" s="115"/>
     </row>
@@ -6672,8 +6675,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-obfuscation"),
-"Testing Simple Obfuscation")</f>
-        <v>Testing Simple Obfuscation</v>
+"Testing Obfuscation")</f>
+        <v>Testing Obfuscation</v>
       </c>
       <c r="G13" s="115"/>
     </row>
@@ -6881,8 +6884,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:K85"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="74" zoomScaleNormal="74" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView topLeftCell="A50" zoomScale="74" zoomScaleNormal="74" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -7190,8 +7193,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06d-Testing-Data-Storage.md#testing-local-data-storage"),
-"Testing For Sensitive Data in Local Data Storage")</f>
-        <v>Testing For Sensitive Data in Local Data Storage</v>
+"Testing Local Data Storage")</f>
+        <v>Testing Local Data Storage</v>
       </c>
       <c r="H16" s="110"/>
       <c r="I16" s="115"/>
@@ -7210,8 +7213,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06d-Testing-Data-Storage.md#testing-local-data-storage"),
-"Testing For Sensitive Data in Local Data Storage")</f>
-        <v>Testing For Sensitive Data in Local Data Storage</v>
+"Testing Local Data Storage")</f>
+        <v>Testing Local Data Storage</v>
       </c>
       <c r="H17" s="110"/>
       <c r="I17" s="115"/>
@@ -7234,8 +7237,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06d-Testing-Data-Storage.md#checking-logs-for-sensitive-data"),
-"Testing For Sensitive Data in Logs")</f>
-        <v>Testing For Sensitive Data in Logs</v>
+"Checking Logs for Sensitive Data")</f>
+        <v>Checking Logs for Sensitive Data</v>
       </c>
       <c r="H18" s="110"/>
       <c r="I18" s="115"/>
@@ -7258,8 +7261,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06d-Testing-Data-Storage.md#determining-whether-sensitive-data-is-sent-to-third-parties"),
-"Testing Whether Sensitive Data Is Sent To Third Parties")</f>
-        <v>Testing Whether Sensitive Data Is Sent To Third Parties</v>
+"Determining Whether Sensitive Data Is Sent to Third Parties")</f>
+        <v>Determining Whether Sensitive Data Is Sent to Third Parties</v>
       </c>
       <c r="H19" s="110"/>
       <c r="I19" s="115"/>
@@ -7282,8 +7285,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06d-Testing-Data-Storage.md#finding-sensitive-data-in-the-keyboard-cache"),
-"Testing Whether the Keyboard Cache Is Disabled for Text Input Fields")</f>
-        <v>Testing Whether the Keyboard Cache Is Disabled for Text Input Fields</v>
+"Finding Sensitive Data in the Keyboard Cache")</f>
+        <v>Finding Sensitive Data in the Keyboard Cache</v>
       </c>
       <c r="H20" s="110"/>
       <c r="I20" s="115"/>
@@ -7306,8 +7309,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06d-Testing-Data-Storage.md#determining-whether-sensitive-data-is-exposed-via-ipc-mechanisms"),
-"Testing Whether Sensitive Data Is Exposed via IPC Mechanisms")</f>
-        <v>Testing Whether Sensitive Data Is Exposed via IPC Mechanisms</v>
+"Determining Whether Sensitive Data Is Exposed via IPC Mechanisms")</f>
+        <v>Determining Whether Sensitive Data Is Exposed via IPC Mechanisms</v>
       </c>
       <c r="H21" s="110"/>
       <c r="I21" s="115"/>
@@ -7330,8 +7333,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06d-Testing-Data-Storage.md#checking-for-sensitive-data-disclosed-through-the-user-interface"),
-"Testing for Sensitive Data Disclosure Through the User Interface")</f>
-        <v>Testing for Sensitive Data Disclosure Through the User Interface</v>
+"Checking for Sensitive Data Disclosed Through the User Interface")</f>
+        <v>Checking for Sensitive Data Disclosed Through the User Interface</v>
       </c>
       <c r="H22" s="110"/>
       <c r="I22" s="115"/>
@@ -7354,8 +7357,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06d-Testing-Data-Storage.md#testing-backups-for-sensitive-data"),
-"Testing for Sensitive Data in Backups")</f>
-        <v>Testing for Sensitive Data in Backups</v>
+"Testing Backups for Sensitive Data")</f>
+        <v>Testing Backups for Sensitive Data</v>
       </c>
       <c r="H23" s="110"/>
       <c r="I23" s="115"/>
@@ -7378,8 +7381,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06d-Testing-Data-Storage.md#testing-auto-generated-screenshots-for-sensitive-information"),
-"Testing for Sensitive Information in Auto-Generated Screenshots")</f>
-        <v>Testing for Sensitive Information in Auto-Generated Screenshots</v>
+"Testing Auto-Generated Screenshots for Sensitive Information")</f>
+        <v>Testing Auto-Generated Screenshots for Sensitive Information</v>
       </c>
       <c r="H24" s="110"/>
       <c r="I24" s="115"/>
@@ -7402,8 +7405,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06d-Testing-Data-Storage.md#testing-memory-for-sensitive-data"),
-"Testing for Sensitive Data in Memory")</f>
-        <v>Testing for Sensitive Data in Memory</v>
+"Testing Memory for Sensitive Data")</f>
+        <v>Testing Memory for Sensitive Data</v>
       </c>
       <c r="H25" s="110"/>
       <c r="I25" s="115"/>
@@ -7426,8 +7429,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06f-Testing-Local-Authentication.md#local-authentication-on-ios"),
-"Testing Local Authentication")</f>
-        <v>Testing Local Authentication</v>
+"Local Authentication on iOS")</f>
+        <v>Local Authentication on iOS</v>
       </c>
       <c r="H26" s="110"/>
       <c r="I26" s="115"/>
@@ -7451,8 +7454,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04i-Testing-user-interaction.md#testing-user-education"),
-"Testing user education")</f>
-        <v>Testing user education</v>
+"Testing User Education")</f>
+        <v>Testing User Education</v>
       </c>
       <c r="H27" s="110"/>
       <c r="I27" s="115"/>
@@ -7490,8 +7493,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06e-Testing-Cryptography.md#testing-key-management"),
-"Verifying Key Management")</f>
-        <v>Verifying Key Management</v>
+"Testing Key Management")</f>
+        <v>Testing Key Management</v>
       </c>
       <c r="H29" s="110"/>
       <c r="I29" s="115"/>
@@ -7514,8 +7517,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04g-Testing-Cryptography.md#custom-implementations-of-cryptography"),
-"Testing for Custom Implementations of Cryptography")</f>
-        <v>Testing for Custom Implementations of Cryptography</v>
+"Custom Implementations of Cryptography")</f>
+        <v>Custom Implementations of Cryptography</v>
       </c>
       <c r="H30" s="110"/>
       <c r="I30" s="115"/>
@@ -7562,8 +7565,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04g-Testing-Cryptography.md#identifying-insecure-andor-deprecated-cryptographic-algorithms"),
-"Testing for Insecure and/or Deprecated Cryptographic Algorithms")</f>
-        <v>Testing for Insecure and/or Deprecated Cryptographic Algorithms</v>
+"Identifying Insecure and/or Deprecated Cryptographic Algorithms")</f>
+        <v>Identifying Insecure and/or Deprecated Cryptographic Algorithms</v>
       </c>
       <c r="H32" s="110"/>
       <c r="I32" s="115"/>
@@ -7586,8 +7589,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06e-Testing-Cryptography.md#testing-key-management"),
-"Verifying Key Management")</f>
-        <v>Verifying Key Management</v>
+"Testing Key Management")</f>
+        <v>Testing Key Management</v>
       </c>
       <c r="H33" s="110"/>
       <c r="I33" s="115"/>
@@ -7648,8 +7651,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04e-Testing-Authentication-and-Session-Management.md#testing-authentication"),
-"Verifying that Users Are Properly Authenticated")</f>
-        <v>Verifying that Users Are Properly Authenticated</v>
+"Testing Authentication")</f>
+        <v>Testing Authentication</v>
       </c>
       <c r="H36" s="110"/>
       <c r="I36" s="115"/>
@@ -7696,8 +7699,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04e-Testing-Authentication-and-Session-Management.md#testing-stateless-token-based-authentication"),
-"Testing Stateless Authentication")</f>
-        <v>Testing Stateless Authentication</v>
+"Testing Stateless (Token-Based) Authentication")</f>
+        <v>Testing Stateless (Token-Based) Authentication</v>
       </c>
       <c r="H38" s="110"/>
       <c r="I38" s="115"/>
@@ -7717,8 +7720,8 @@
 CONCATENATE(
 BASE_URL,
 "0x04e-Testing-Authentication-and-Session-Management.md#user-logout-and-session-timeouts"),
-"Testing the Logout Functionality")</f>
-        <v>Testing the Logout Functionality</v>
+"User Logout and Session Timeouts")</f>
+        <v>User Logout and Session Timeouts</v>
       </c>
       <c r="H39" s="110"/>
       <c r="I39" s="115"/>
@@ -7742,8 +7745,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04e-Testing-Authentication-and-Session-Management.md#best-practices-for-passwords"),
-"Testing the Password Policy")</f>
-        <v>Testing the Password Policy</v>
+"Best Practices for Passwords")</f>
+        <v>Best Practices for Passwords</v>
       </c>
       <c r="H40" s="110"/>
       <c r="I40" s="115"/>
@@ -7767,8 +7770,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04e-Testing-Authentication-and-Session-Management.md#running-a-password-dictionary-attack"),
-"Testing Excessive Login Attempts")</f>
-        <v>Testing Excessive Login Attempts</v>
+"Running a Password Dictionary Attack")</f>
+        <v>Running a Password Dictionary Attack</v>
       </c>
       <c r="H41" s="110"/>
       <c r="I41" s="115"/>
@@ -7791,8 +7794,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04e-Testing-Authentication-and-Session-Management.md#session-timeout"),
-"Testing the Session Timeout")</f>
-        <v>Testing the Session Timeout</v>
+"Session Timeout")</f>
+        <v>Session Timeout</v>
       </c>
       <c r="H42" s="99"/>
       <c r="I42" s="117"/>
@@ -7815,8 +7818,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06f-Testing-Local-Authentication.md#testing-local-authentication"),
-"Testing Biometric Authentication")</f>
-        <v>Testing Biometric Authentication</v>
+"Testing Local Authentication")</f>
+        <v>Testing Local Authentication</v>
       </c>
       <c r="H43" s="110"/>
       <c r="I43" s="115"/>
@@ -7839,8 +7842,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04e-Testing-Authentication-and-Session-Management.md#verifying-that-2fa-is-enforced"),
-"Testing 2-Factor Authentication")</f>
-        <v>Testing 2-Factor Authentication</v>
+"Verifying that 2FA is Enforced")</f>
+        <v>Verifying that 2FA is Enforced</v>
       </c>
       <c r="H44" s="110"/>
       <c r="I44" s="115"/>
@@ -7863,8 +7866,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04e-Testing-Authentication-and-Session-Management.md#2-factor-authentication-and-step-up-authentication"),
-"Testing Step-up Authentication")</f>
-        <v>Testing Step-up Authentication</v>
+"2-Factor Authentication and Step-up Authentication")</f>
+        <v>2-Factor Authentication and Step-up Authentication</v>
       </c>
       <c r="H45" s="110"/>
       <c r="I45" s="115"/>
@@ -7887,8 +7890,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04e-Testing-Authentication-and-Session-Management.md#login-activity-and-device-blocking"),
-"Testing Login Activity and Device Blocking")</f>
-        <v>Testing Login Activity and Device Blocking</v>
+"Login Activity and Device Blocking")</f>
+        <v>Login Activity and Device Blocking</v>
       </c>
       <c r="H46" s="110"/>
       <c r="I46" s="115"/>
@@ -7925,15 +7928,15 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04f-Testing-Network-Communication.md#verifying-data-encryption-on-the-network"),
-"Testing for Unencrypted Sensitive Data on the Network")</f>
-        <v>Testing for Unencrypted Sensitive Data on the Network</v>
+"Verifying Data Encryption on the Network")</f>
+        <v>Verifying Data Encryption on the Network</v>
       </c>
       <c r="H48" s="98" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06g-Testing-Network-Communication.md#app-transport-security"),
-"App Transport Security (ATS)")</f>
-        <v>App Transport Security (ATS)</v>
+"App Transport Security")</f>
+        <v>App Transport Security</v>
       </c>
       <c r="I48" s="120"/>
     </row>
@@ -7955,15 +7958,15 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04f-Testing-Network-Communication.md#recommended-tls-settings"),
-"Verifying the TLS Settings")</f>
-        <v>Verifying the TLS Settings</v>
+"Recommended TLS Settings")</f>
+        <v>Recommended TLS Settings</v>
       </c>
       <c r="H49" s="98" t="str">
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06g-Testing-Network-Communication.md#app-transport-security"),
-"App Transport Security (ATS)")</f>
-        <v>App Transport Security (ATS)</v>
+"App Transport Security")</f>
+        <v>App Transport Security</v>
       </c>
       <c r="I49" s="120"/>
     </row>
@@ -7985,8 +7988,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06g-Testing-Network-Communication.md#testing-custom-certificate-stores-and-certificate-pinning"),
-"Testing Custom Certificate Stores and SSL Pinning")</f>
-        <v>Testing Custom Certificate Stores and SSL Pinning</v>
+"Testing Custom Certificate Stores and Certificate Pinning")</f>
+        <v>Testing Custom Certificate Stores and Certificate Pinning</v>
       </c>
       <c r="H50" s="98"/>
       <c r="I50" s="120"/>
@@ -8009,8 +8012,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06g-Testing-Network-Communication.md#testing-custom-certificate-stores-and-certificate-pinning"),
-"Testing Custom Certificate Stores and SSL Pinning")</f>
-        <v>Testing Custom Certificate Stores and SSL Pinning</v>
+"Testing Custom Certificate Stores and Certificate Pinning")</f>
+        <v>Testing Custom Certificate Stores and Certificate Pinning</v>
       </c>
       <c r="H51" s="110"/>
       <c r="I51" s="115"/>
@@ -8033,8 +8036,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04f-Testing-Network-Communication.md#making-sure-that-critical-operations-use-secure-communication-channels"),
-"Verifying that Critical Operations Use Secure Communication Channels")</f>
-        <v>Verifying that Critical Operations Use Secure Communication Channels</v>
+"Making Sure that Critical Operations Use Secure Communication Channels")</f>
+        <v>Making Sure that Critical Operations Use Secure Communication Channels</v>
       </c>
       <c r="H52" s="110"/>
       <c r="I52" s="115"/>
@@ -8119,8 +8122,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x04h-Testing-Code-Quality.md#injection-flaws"),
-"Testing Input Validation and Sanitization")</f>
-        <v>Testing Input Validation and Sanitization</v>
+"Injection Flaws")</f>
+        <v>Injection Flaws</v>
       </c>
       <c r="H56" s="110"/>
       <c r="I56" s="115"/>
@@ -8167,8 +8170,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06h-Testing-Platform-Interaction.md#testing-for-sensitive-functionality-exposure-through-ipc"),
-"Testing For Sensitive Functionality Exposure Through IPC")</f>
-        <v>Testing For Sensitive Functionality Exposure Through IPC</v>
+"Testing for Sensitive Functionality Exposure Through IPC")</f>
+        <v>Testing for Sensitive Functionality Exposure Through IPC</v>
       </c>
       <c r="H58" s="110"/>
       <c r="I58" s="115"/>
@@ -8191,8 +8194,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06h-Testing-Platform-Interaction.md#testing-ios-webviews"),
-"Testing JavaScript Execution in WebViews")</f>
-        <v>Testing JavaScript Execution in WebViews</v>
+"Testing iOS WebViews")</f>
+        <v>Testing iOS WebViews</v>
       </c>
       <c r="H59" s="110"/>
       <c r="I59" s="115"/>
@@ -8239,8 +8242,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06h-Testing-Platform-Interaction.md#determining-whether-native-methods-are-exposed-through-webviews"),
-"Testing Whether Native Methods Are Exposed Through WebViews")</f>
-        <v>Testing Whether Native Methods Are Exposed Through WebViews</v>
+"Determining Whether Native Methods Are Exposed Through WebViews")</f>
+        <v>Determining Whether Native Methods Are Exposed Through WebViews</v>
       </c>
       <c r="H61" s="110"/>
       <c r="I61" s="115"/>
@@ -8263,8 +8266,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06h-Testing-Platform-Interaction.md#testing-object-persistence"),
-"Testing Object (De-)Serialization")</f>
-        <v>Testing Object (De-)Serialization</v>
+"Testing Object Persistence")</f>
+        <v>Testing Object Persistence</v>
       </c>
       <c r="H62" s="110"/>
       <c r="I62" s="115"/>
@@ -8301,8 +8304,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06i-Testing-Code-Quality-and-Build-Settings.md#making-sure-that-the-app-is-properly-signed"),
-"Verifying That the App is Properly Signed")</f>
-        <v>Verifying That the App is Properly Signed</v>
+"Making Sure that the App Is Properly Signed")</f>
+        <v>Making Sure that the App Is Properly Signed</v>
       </c>
       <c r="H64" s="110"/>
       <c r="I64" s="115"/>
@@ -8325,8 +8328,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06i-Testing-Code-Quality-and-Build-Settings.md#determining-whether-the-app-is-debuggable"),
-"Testing If the App is Debuggable")</f>
-        <v>Testing If the App is Debuggable</v>
+"Determining Whether the App is Debuggable")</f>
+        <v>Determining Whether the App is Debuggable</v>
       </c>
       <c r="H65" s="110"/>
       <c r="I65" s="115"/>
@@ -8349,8 +8352,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06i-Testing-Code-Quality-and-Build-Settings.md#finding-debugging-symbols"),
-"Testing for Debugging Symbols")</f>
-        <v>Testing for Debugging Symbols</v>
+"Finding Debugging Symbols")</f>
+        <v>Finding Debugging Symbols</v>
       </c>
       <c r="H66" s="110"/>
       <c r="I66" s="115"/>
@@ -8373,8 +8376,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06i-Testing-Code-Quality-and-Build-Settings.md#finding-debugging-code-and-verbose-error-logging"),
-"Testing for Debugging Code and Verbose Error Logging")</f>
-        <v>Testing for Debugging Code and Verbose Error Logging</v>
+"Finding Debugging Code and Verbose Error Logging")</f>
+        <v>Finding Debugging Code and Verbose Error Logging</v>
       </c>
       <c r="H67" s="110"/>
       <c r="I67" s="115"/>
@@ -8397,8 +8400,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06i-Testing-Code-Quality-and-Build-Settings.md#checking-for-weaknesses-in-third-party-libraries"),
-"Testing for Weaknesses in Third Party Libraries")</f>
-        <v>Testing for Weaknesses in Third Party Libraries</v>
+"Checking for Weaknesses in Third Party Libraries")</f>
+        <v>Checking for Weaknesses in Third Party Libraries</v>
       </c>
       <c r="H68" s="110"/>
       <c r="I68" s="115"/>
@@ -8445,8 +8448,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06i-Testing-Code-Quality-and-Build-Settings.md#testing-exception-handling"),
-"Testing  Error Handling in Security Controls")</f>
-        <v>Testing  Error Handling in Security Controls</v>
+"Testing Exception Handling")</f>
+        <v>Testing Exception Handling</v>
       </c>
       <c r="H70" s="110"/>
       <c r="I70" s="115"/>
@@ -8469,8 +8472,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06i-Testing-Code-Quality-and-Build-Settings.md#memory-corruption-bugs"),
-"Testing for Memory Management Bugs")</f>
-        <v>Testing for Memory Management Bugs</v>
+"Memory Corruption Bugs")</f>
+        <v>Memory Corruption Bugs</v>
       </c>
       <c r="H71" s="110"/>
       <c r="I71" s="115"/>
@@ -8493,8 +8496,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06i-Testing-Code-Quality-and-Build-Settings.md#make-sure-that-free-security-features-are-activated"),
-"Verifying usage of Free Security Features")</f>
-        <v>Verifying usage of Free Security Features</v>
+"Make Sure That Free Security Features Are Activated")</f>
+        <v>Make Sure That Free Security Features Are Activated</v>
       </c>
       <c r="H72" s="110"/>
       <c r="I72" s="115"/>
@@ -8679,8 +8682,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="B1:G32"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -8750,8 +8753,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#jailbreak-detection"),
-"Testing Jailbreak Detection")</f>
-        <v>Testing Jailbreak Detection</v>
+"Jailbreak Detection")</f>
+        <v>Jailbreak Detection</v>
       </c>
       <c r="G5" s="115"/>
     </row>
@@ -8772,8 +8775,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#anti-debugging-checks"),
-"Testing Debugging Defenses")</f>
-        <v>Testing Debugging Defenses</v>
+"Anti-Debugging Checks")</f>
+        <v>Anti-Debugging Checks</v>
       </c>
       <c r="G6" s="115"/>
     </row>
@@ -8794,8 +8797,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#file-integrity-checks"),
-"Testing File Integrity Checks")</f>
-        <v>Testing File Integrity Checks</v>
+"File Integrity Checks")</f>
+        <v>File Integrity Checks</v>
       </c>
       <c r="G7" s="115"/>
     </row>
@@ -8934,8 +8937,8 @@
         <f>HYPERLINK(CONCATENATE(
 BASE_URL,
 "0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#device-binding"),
-"Testing Device Binding")</f>
-        <v>Testing Device Binding</v>
+"Device Binding")</f>
+        <v>Device Binding</v>
       </c>
       <c r="G15" s="115"/>
     </row>
@@ -9166,10 +9169,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -9538,6 +9541,23 @@
         <v>287</v>
       </c>
     </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="52" t="s">
+        <v>259</v>
+      </c>
+      <c r="B24" s="87" t="s">
+        <v>285</v>
+      </c>
+      <c r="C24" s="132" t="s">
+        <v>279</v>
+      </c>
+      <c r="D24" s="43">
+        <v>43674</v>
+      </c>
+      <c r="E24" s="92" t="s">
+        <v>288</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Synchronizing excel links description in the French version with the mstg
</commit_message>
<xml_diff>
--- a/Checklists/Mobile_App_Security_Checklist-English_1.1.xlsx
+++ b/Checklists/Mobile_App_Security_Checklist-English_1.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abderrahmane.LAPTOP-NBPOQCF6\Personal\R&amp;D\OWASP\MSTG\owasp-mstg\Checklists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AB9F59-A106-4ABC-ACAF-F77A669F022F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED238C0-E81D-4218-AB2D-EC0183621E9E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="6" r:id="rId1"/>
@@ -2187,85 +2187,121 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2280,42 +2316,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3655,48 +3655,48 @@
   <sheetData>
     <row r="1" spans="2:4" ht="8" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B2" s="144" t="s">
+      <c r="B2" s="137" t="s">
         <v>219</v>
       </c>
-      <c r="C2" s="145"/>
-      <c r="D2" s="146"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="139"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B3" s="147"/>
-      <c r="C3" s="148"/>
-      <c r="D3" s="149"/>
+      <c r="B3" s="140"/>
+      <c r="C3" s="141"/>
+      <c r="D3" s="142"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="147"/>
-      <c r="C4" s="148"/>
-      <c r="D4" s="149"/>
+      <c r="B4" s="140"/>
+      <c r="C4" s="141"/>
+      <c r="D4" s="142"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="147"/>
-      <c r="C5" s="148"/>
-      <c r="D5" s="149"/>
+      <c r="B5" s="140"/>
+      <c r="C5" s="141"/>
+      <c r="D5" s="142"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B6" s="147"/>
-      <c r="C6" s="148"/>
-      <c r="D6" s="149"/>
+      <c r="B6" s="140"/>
+      <c r="C6" s="141"/>
+      <c r="D6" s="142"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B7" s="147"/>
-      <c r="C7" s="148"/>
-      <c r="D7" s="149"/>
+      <c r="B7" s="140"/>
+      <c r="C7" s="141"/>
+      <c r="D7" s="142"/>
     </row>
     <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="150"/>
-      <c r="C8" s="151"/>
-      <c r="D8" s="152"/>
+      <c r="B8" s="143"/>
+      <c r="C8" s="144"/>
+      <c r="D8" s="145"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B9" s="153" t="s">
+      <c r="B9" s="146" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="140"/>
-      <c r="D9" s="141"/>
+      <c r="C9" s="147"/>
+      <c r="D9" s="148"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="126" t="s">
@@ -3706,19 +3706,19 @@
       <c r="D10" s="128"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B11" s="159" t="s">
+      <c r="B11" s="154" t="s">
         <v>278</v>
       </c>
-      <c r="C11" s="159"/>
+      <c r="C11" s="154"/>
       <c r="D11" s="129" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B12" s="133" t="s">
+      <c r="B12" s="135" t="s">
         <v>280</v>
       </c>
-      <c r="C12" s="143"/>
+      <c r="C12" s="136"/>
       <c r="D12" s="130" t="str">
         <f>HYPERLINK(CONCATENATE(
 "https://github.com/OWASP/owasp-masvs/blob/",
@@ -3728,19 +3728,19 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B13" s="154" t="s">
+      <c r="B13" s="149" t="s">
         <v>277</v>
       </c>
-      <c r="C13" s="155"/>
+      <c r="C13" s="150"/>
       <c r="D13" s="12" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B14" s="133" t="s">
+      <c r="B14" s="135" t="s">
         <v>221</v>
       </c>
-      <c r="C14" s="143"/>
+      <c r="C14" s="136"/>
       <c r="D14" s="124" t="str">
         <f>HYPERLINK(CONCATENATE(
 "https://github.com/OWASP/owasp-mstg/blob/",
@@ -3750,69 +3750,69 @@
       </c>
     </row>
     <row r="15" spans="2:4" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="156" t="s">
+      <c r="B15" s="151" t="s">
         <v>263</v>
       </c>
-      <c r="C15" s="157"/>
-      <c r="D15" s="158"/>
+      <c r="C15" s="152"/>
+      <c r="D15" s="153"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B16" s="138" t="s">
+      <c r="B16" s="133" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="139"/>
+      <c r="C16" s="134"/>
       <c r="D16" s="12"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="133" t="s">
+      <c r="B17" s="135" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="143"/>
+      <c r="C17" s="136"/>
       <c r="D17" s="12"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="138" t="s">
+      <c r="B18" s="133" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="139"/>
+      <c r="C18" s="134"/>
       <c r="D18" s="12"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="138" t="s">
+      <c r="B19" s="133" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="139"/>
+      <c r="C19" s="134"/>
       <c r="D19" s="12"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="138" t="s">
+      <c r="B20" s="133" t="s">
         <v>135</v>
       </c>
-      <c r="C20" s="139"/>
+      <c r="C20" s="134"/>
       <c r="D20" s="12"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21" s="138" t="s">
+      <c r="B21" s="133" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="139"/>
+      <c r="C21" s="134"/>
       <c r="D21" s="12" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="138" t="s">
+      <c r="B22" s="133" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="139"/>
+      <c r="C22" s="134"/>
       <c r="D22" s="12" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B23" s="140"/>
-      <c r="C23" s="140"/>
-      <c r="D23" s="141"/>
+      <c r="B23" s="147"/>
+      <c r="C23" s="147"/>
+      <c r="D23" s="148"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
@@ -3829,37 +3829,37 @@
       <c r="D25" s="12"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B26" s="138" t="s">
+      <c r="B26" s="133" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="139"/>
+      <c r="C26" s="134"/>
       <c r="D26" s="12"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B27" s="138" t="s">
+      <c r="B27" s="133" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="139"/>
+      <c r="C27" s="134"/>
       <c r="D27" s="12"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B28" s="138" t="s">
+      <c r="B28" s="133" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="139"/>
+      <c r="C28" s="134"/>
       <c r="D28" s="12"/>
     </row>
     <row r="29" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="142" t="s">
+      <c r="B29" s="159" t="s">
         <v>257</v>
       </c>
-      <c r="C29" s="139"/>
+      <c r="C29" s="134"/>
       <c r="D29" s="12"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B30" s="140"/>
-      <c r="C30" s="140"/>
-      <c r="D30" s="141"/>
+      <c r="B30" s="147"/>
+      <c r="C30" s="147"/>
+      <c r="D30" s="148"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
@@ -3876,37 +3876,37 @@
       <c r="D32" s="12"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B33" s="138" t="s">
+      <c r="B33" s="133" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="139"/>
+      <c r="C33" s="134"/>
       <c r="D33" s="12"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B34" s="138" t="s">
+      <c r="B34" s="133" t="s">
         <v>99</v>
       </c>
-      <c r="C34" s="139"/>
+      <c r="C34" s="134"/>
       <c r="D34" s="12"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B35" s="138" t="s">
+      <c r="B35" s="133" t="s">
         <v>100</v>
       </c>
-      <c r="C35" s="139"/>
+      <c r="C35" s="134"/>
       <c r="D35" s="12"/>
     </row>
     <row r="36" spans="2:4" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="142" t="s">
+      <c r="B36" s="159" t="s">
         <v>258</v>
       </c>
-      <c r="C36" s="139"/>
+      <c r="C36" s="134"/>
       <c r="D36" s="12"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B37" s="140"/>
-      <c r="C37" s="140"/>
-      <c r="D37" s="141"/>
+      <c r="B37" s="147"/>
+      <c r="C37" s="147"/>
+      <c r="D37" s="148"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
@@ -3916,100 +3916,97 @@
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B39" s="135"/>
-      <c r="C39" s="136"/>
-      <c r="D39" s="137"/>
+      <c r="B39" s="155"/>
+      <c r="C39" s="156"/>
+      <c r="D39" s="157"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B40" s="133" t="s">
+      <c r="B40" s="135" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="134"/>
+      <c r="C40" s="158"/>
       <c r="D40" s="39"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B41" s="133" t="s">
+      <c r="B41" s="135" t="s">
         <v>92</v>
       </c>
-      <c r="C41" s="134"/>
+      <c r="C41" s="158"/>
       <c r="D41" s="39"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B42" s="133" t="s">
+      <c r="B42" s="135" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="134"/>
+      <c r="C42" s="158"/>
       <c r="D42" s="39"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B43" s="133" t="s">
+      <c r="B43" s="135" t="s">
         <v>94</v>
       </c>
-      <c r="C43" s="134"/>
+      <c r="C43" s="158"/>
       <c r="D43" s="40"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B44" s="133" t="s">
+      <c r="B44" s="135" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="134"/>
+      <c r="C44" s="158"/>
       <c r="D44" s="39"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B45" s="135"/>
-      <c r="C45" s="136"/>
-      <c r="D45" s="137"/>
+      <c r="B45" s="155"/>
+      <c r="C45" s="156"/>
+      <c r="D45" s="157"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B46" s="133" t="s">
+      <c r="B46" s="135" t="s">
         <v>91</v>
       </c>
-      <c r="C46" s="134"/>
+      <c r="C46" s="158"/>
       <c r="D46" s="39"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B47" s="133" t="s">
+      <c r="B47" s="135" t="s">
         <v>92</v>
       </c>
-      <c r="C47" s="134"/>
+      <c r="C47" s="158"/>
       <c r="D47" s="39"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B48" s="133" t="s">
+      <c r="B48" s="135" t="s">
         <v>93</v>
       </c>
-      <c r="C48" s="134"/>
+      <c r="C48" s="158"/>
       <c r="D48" s="39"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B49" s="133" t="s">
+      <c r="B49" s="135" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="134"/>
+      <c r="C49" s="158"/>
       <c r="D49" s="40"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B50" s="133" t="s">
+      <c r="B50" s="135" t="s">
         <v>95</v>
       </c>
-      <c r="C50" s="134"/>
+      <c r="C50" s="158"/>
       <c r="D50" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B2:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:C46"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B39:D39"/>
@@ -4024,16 +4021,19 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B2:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4080,11 +4080,11 @@
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="2:24" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="164"/>
-      <c r="C4" s="164"/>
-      <c r="D4" s="164"/>
-      <c r="E4" s="164"/>
-      <c r="F4" s="164"/>
+      <c r="B4" s="176"/>
+      <c r="C4" s="176"/>
+      <c r="D4" s="176"/>
+      <c r="E4" s="176"/>
+      <c r="F4" s="176"/>
     </row>
     <row r="5" spans="2:24" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="20"/>
@@ -4099,16 +4099,16 @@
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
-      <c r="G6" s="174" t="s">
+      <c r="G6" s="160" t="s">
         <v>117</v>
       </c>
-      <c r="H6" s="175"/>
-      <c r="I6" s="176"/>
-      <c r="V6" s="174" t="s">
+      <c r="H6" s="161"/>
+      <c r="I6" s="162"/>
+      <c r="V6" s="160" t="s">
         <v>117</v>
       </c>
-      <c r="W6" s="175"/>
-      <c r="X6" s="176"/>
+      <c r="W6" s="161"/>
+      <c r="X6" s="162"/>
     </row>
     <row r="7" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="13"/>
@@ -4123,18 +4123,18 @@
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
-      <c r="G8" s="165">
+      <c r="G8" s="163">
         <f>AVERAGE(G43:G50)*5</f>
         <v>0</v>
       </c>
-      <c r="H8" s="166"/>
-      <c r="I8" s="167"/>
-      <c r="V8" s="165">
+      <c r="H8" s="164"/>
+      <c r="I8" s="165"/>
+      <c r="V8" s="163">
         <f>AVERAGE(K43:K50)*5</f>
         <v>0</v>
       </c>
-      <c r="W8" s="166"/>
-      <c r="X8" s="167"/>
+      <c r="W8" s="164"/>
+      <c r="X8" s="165"/>
     </row>
     <row r="9" spans="2:24" ht="91" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="21"/>
@@ -4142,12 +4142,12 @@
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
-      <c r="G9" s="168"/>
-      <c r="H9" s="169"/>
-      <c r="I9" s="170"/>
-      <c r="V9" s="168"/>
-      <c r="W9" s="169"/>
-      <c r="X9" s="170"/>
+      <c r="G9" s="166"/>
+      <c r="H9" s="167"/>
+      <c r="I9" s="168"/>
+      <c r="V9" s="166"/>
+      <c r="W9" s="167"/>
+      <c r="X9" s="168"/>
     </row>
     <row r="10" spans="2:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="13"/>
@@ -4155,12 +4155,12 @@
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="168"/>
-      <c r="H10" s="169"/>
-      <c r="I10" s="170"/>
-      <c r="V10" s="168"/>
-      <c r="W10" s="169"/>
-      <c r="X10" s="170"/>
+      <c r="G10" s="166"/>
+      <c r="H10" s="167"/>
+      <c r="I10" s="168"/>
+      <c r="V10" s="166"/>
+      <c r="W10" s="167"/>
+      <c r="X10" s="168"/>
     </row>
     <row r="11" spans="2:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="13"/>
@@ -4168,19 +4168,19 @@
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="171"/>
-      <c r="H11" s="172"/>
-      <c r="I11" s="173"/>
-      <c r="V11" s="171"/>
-      <c r="W11" s="172"/>
-      <c r="X11" s="173"/>
+      <c r="G11" s="169"/>
+      <c r="H11" s="170"/>
+      <c r="I11" s="171"/>
+      <c r="V11" s="169"/>
+      <c r="W11" s="170"/>
+      <c r="X11" s="171"/>
     </row>
     <row r="12" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="160"/>
-      <c r="C12" s="160"/>
-      <c r="D12" s="160"/>
-      <c r="E12" s="160"/>
-      <c r="F12" s="160"/>
+      <c r="B12" s="172"/>
+      <c r="C12" s="172"/>
+      <c r="D12" s="172"/>
+      <c r="E12" s="172"/>
+      <c r="F12" s="172"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
@@ -4204,11 +4204,11 @@
       <c r="F15" s="13"/>
     </row>
     <row r="16" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="160"/>
-      <c r="C16" s="160"/>
-      <c r="D16" s="160"/>
-      <c r="E16" s="160"/>
-      <c r="F16" s="160"/>
+      <c r="B16" s="172"/>
+      <c r="C16" s="172"/>
+      <c r="D16" s="172"/>
+      <c r="E16" s="172"/>
+      <c r="F16" s="172"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="14"/>
@@ -4261,18 +4261,18 @@
     </row>
     <row r="35" spans="3:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="3:11" ht="14.5" x14ac:dyDescent="0.3">
-      <c r="D41" s="161" t="s">
+      <c r="D41" s="173" t="s">
         <v>115</v>
       </c>
-      <c r="E41" s="162"/>
-      <c r="F41" s="162"/>
-      <c r="G41" s="163"/>
-      <c r="H41" s="161" t="s">
+      <c r="E41" s="174"/>
+      <c r="F41" s="174"/>
+      <c r="G41" s="175"/>
+      <c r="H41" s="173" t="s">
         <v>116</v>
       </c>
-      <c r="I41" s="162"/>
-      <c r="J41" s="162"/>
-      <c r="K41" s="163"/>
+      <c r="I41" s="174"/>
+      <c r="J41" s="174"/>
+      <c r="K41" s="175"/>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.3">
       <c r="D42" s="17" t="s">
@@ -4598,15 +4598,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G8:I11"/>
+    <mergeCell ref="G6:I6"/>
     <mergeCell ref="V6:X6"/>
     <mergeCell ref="V8:X11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="D41:G41"/>
     <mergeCell ref="H41:K41"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G8:I11"/>
-    <mergeCell ref="G6:I6"/>
   </mergeCells>
   <conditionalFormatting sqref="F14">
     <cfRule type="iconSet" priority="3">
@@ -4647,8 +4647,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:K85"/>
   <sheetViews>
-    <sheetView topLeftCell="B44" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="B50" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -5032,7 +5032,7 @@
       <c r="H19" s="97"/>
       <c r="I19" s="115"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" ht="31" x14ac:dyDescent="0.35">
       <c r="B20" s="68" t="s">
         <v>50</v>
       </c>
@@ -5056,7 +5056,7 @@
       <c r="H20" s="97"/>
       <c r="I20" s="115"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" ht="31" x14ac:dyDescent="0.35">
       <c r="B21" s="68" t="s">
         <v>13</v>
       </c>
@@ -5769,7 +5769,7 @@
       <c r="H51" s="97"/>
       <c r="I51" s="115"/>
     </row>
-    <row r="52" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:9" ht="31" x14ac:dyDescent="0.35">
       <c r="B52" s="68" t="s">
         <v>35</v>
       </c>
@@ -6407,7 +6407,7 @@
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="G3:H3"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F74:F1048576 I74:I1048576" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Yes,No,N/A"</formula1>
     </dataValidation>
@@ -6556,7 +6556,7 @@
       </c>
       <c r="G7" s="115"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:7" ht="31" x14ac:dyDescent="0.35">
       <c r="B8" s="70" t="s">
         <v>237</v>
       </c>
@@ -8018,7 +8018,7 @@
       <c r="H51" s="110"/>
       <c r="I51" s="115"/>
     </row>
-    <row r="52" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:9" ht="31" x14ac:dyDescent="0.35">
       <c r="B52" s="68" t="s">
         <v>35</v>
       </c>
@@ -9171,7 +9171,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>

</xml_diff>